<commit_message>
fix problems found by students, use different color to highlight different pillars, make the link of faculty to open new tab
</commit_message>
<xml_diff>
--- a/data_script/dku_knowledge_230504.xlsx
+++ b/data_script/dku_knowledge_230504.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sd540\Desktop\Division Portal\Interdisciplinary-Knowledge-Map-DKU\data_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA3043A-232D-4DE2-A71D-52C977E55A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFD3813-E127-49CA-8E06-E302228B04EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>Data and computer sciences</t>
   </si>
   <si>
-    <t>Biological, Behavioral sciences and Health</t>
-  </si>
-  <si>
     <t xml:space="preserve">MATHEMATICS, INTERDISCIPLINARY APPLICATIONS;  BIOPHYSICS; </t>
   </si>
   <si>
@@ -533,9 +530,6 @@
     <t>MACHINE LEARNING</t>
   </si>
   <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
     <t>Ming-chun Huang</t>
   </si>
   <si>
@@ -1653,6 +1647,12 @@
   </si>
   <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/feng-tian/</t>
+  </si>
+  <si>
+    <t>Biological, behavioral sciences and health</t>
+  </si>
+  <si>
+    <t>Computer science</t>
   </si>
 </sst>
 </file>
@@ -2604,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,13 +2856,13 @@
         <v>57</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V4" s="6" t="s">
         <v>38</v>
@@ -2882,40 +2882,40 @@
         <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="K5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V5" s="6" t="s">
         <v>38</v>
@@ -2935,34 +2935,34 @@
         <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="K6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>35</v>
@@ -2971,7 +2971,7 @@
         <v>57</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V6" s="6" t="s">
         <v>38</v>
@@ -2991,49 +2991,49 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>36</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V7" s="6" t="s">
         <v>38</v>
@@ -3053,31 +3053,31 @@
         <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="K8" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>35</v>
@@ -3086,10 +3086,10 @@
         <v>57</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V8" s="6" t="s">
         <v>38</v>
@@ -3109,37 +3109,37 @@
         <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="M9" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="N9" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>35</v>
@@ -3148,10 +3148,10 @@
         <v>57</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V9" s="6" t="s">
         <v>38</v>
@@ -3171,13 +3171,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>41</v>
@@ -3186,25 +3186,25 @@
         <v>29</v>
       </c>
       <c r="K10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V10" s="6" t="s">
         <v>38</v>
@@ -3224,49 +3224,49 @@
         <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L11" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N11" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>38</v>
@@ -3286,40 +3286,40 @@
         <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="L12" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>126</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N12" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>35</v>
@@ -3328,10 +3328,10 @@
         <v>57</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="V12" s="6" t="s">
         <v>38</v>
@@ -3340,7 +3340,7 @@
         <v>24</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3354,46 +3354,46 @@
         <v>25</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="K13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="L13" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="M13" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="O13" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>38</v>
@@ -3410,55 +3410,55 @@
         <v>57</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="K14" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="L14" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N14" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>57</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="R14" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="U14" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="T14" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="U14" s="6" t="s">
+      <c r="V14" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="V14" s="6" t="s">
-        <v>148</v>
-      </c>
       <c r="W14" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3469,46 +3469,46 @@
         <v>57</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="K15" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="L15" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="M15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N15" s="6" t="s">
+      <c r="O15" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3519,52 +3519,52 @@
         <v>57</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>537</v>
-      </c>
-      <c r="M16" s="6" t="s">
+      <c r="N16" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="N16" s="6" t="s">
+      <c r="O16" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U16" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V16" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>164</v>
+        <v>537</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3575,58 +3575,58 @@
         <v>57</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="K17" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="L17" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="V17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>164</v>
+        <v>537</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3637,61 +3637,61 @@
         <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="L18" s="13" t="s">
         <v>176</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>178</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V18" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3702,37 +3702,37 @@
         <v>57</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="G19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="K19" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="L19" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>57</v>
@@ -3741,19 +3741,19 @@
         <v>35</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="V19" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X19" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3764,34 +3764,34 @@
         <v>57</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="M20" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="N20" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M20" s="6" t="s">
+      <c r="O20" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>57</v>
@@ -3800,22 +3800,22 @@
         <v>35</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V20" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>164</v>
+        <v>537</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3826,52 +3826,52 @@
         <v>57</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="L21" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="M21" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="N21" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="O21" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U21" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="V21" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W21" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:24" s="10" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3879,52 +3879,52 @@
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="K22" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="L22" s="15" t="s">
         <v>211</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="L22" s="15" t="s">
-        <v>213</v>
       </c>
       <c r="M22" s="10" t="s">
         <v>32</v>
       </c>
       <c r="N22" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="S22" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="O22" s="10" t="s">
+      <c r="V22" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="P22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="S22" s="10" t="s">
+      <c r="W22" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="V22" s="10" t="s">
+      <c r="X22" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="W22" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="X22" s="10" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3932,55 +3932,55 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F23" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="K23" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="L23" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="L23" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S23" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W23" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="V23" s="6" t="s">
+      <c r="X23" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="W23" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="X23" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3988,52 +3988,52 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="F24" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="L24" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="M24" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="N24" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="M24" s="6" t="s">
+      <c r="O24" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="P24" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="T24" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="O24" s="6" t="s">
+      <c r="V24" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="X24" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S24" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="W24" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="X24" s="6" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4041,58 +4041,58 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="F25" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="K25" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="L25" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N25" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="P25" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="O25" s="6" t="s">
+      <c r="Q25" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S25" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="P25" s="6" t="s">
+      <c r="U25" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="Q25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S25" s="6" t="s">
+      <c r="V25" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="X25" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4100,52 +4100,52 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="K26" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="L26" s="13" t="s">
         <v>251</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>253</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N26" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="V26" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W26" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="O26" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S26" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="V26" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="W26" s="6" t="s">
-        <v>256</v>
-      </c>
       <c r="X26" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4153,58 +4153,58 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K27" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="L27" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N27" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="S27" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="T27" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="O27" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q27" s="6" t="s">
+      <c r="U27" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="S27" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="T27" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="U27" s="6" t="s">
-        <v>247</v>
-      </c>
       <c r="V27" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W27" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="X27" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="W27" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="X27" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4212,64 +4212,64 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="I28" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="K28" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="L28" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>270</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N28" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q28" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S28" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="T28" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="O28" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="P28" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="Q28" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S28" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="T28" s="6" t="s">
-        <v>273</v>
-      </c>
       <c r="V28" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W28" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="X28" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="W28" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="X28" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4277,55 +4277,55 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="L29" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="K29" s="7" t="s">
+      <c r="M29" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="N29" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="M29" s="6" t="s">
+      <c r="O29" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="N29" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="O29" s="6" t="s">
-        <v>280</v>
-      </c>
       <c r="P29" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="V29" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W29" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="X29" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="W29" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="X29" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4333,55 +4333,55 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="F30" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="K30" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="L30" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="K30" s="7" t="s">
+      <c r="M30" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="L30" s="8" t="s">
+      <c r="N30" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="N30" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>287</v>
-      </c>
       <c r="P30" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S30" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="U30" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="V30" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W30" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="U30" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="V30" s="6" t="s">
+      <c r="X30" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="W30" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="X30" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4389,49 +4389,49 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="K31" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="F31" s="6" t="s">
+      <c r="L31" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="M31" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="N31" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="O31" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="N31" s="6" t="s">
+      <c r="P31" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="W31" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="X31" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S31" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="V31" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="W31" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="X31" s="6" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4439,67 +4439,67 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="K32" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="L32" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="M32" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="N32" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="O32" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="P32" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q32" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="R32" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S32" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="T32" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="U32" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="V32" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="T32" s="6" t="s">
+      <c r="W32" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="X32" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="U32" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="V32" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="W32" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4507,55 +4507,55 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="F33" s="6" t="s">
+      <c r="K33" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="L33" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="M33" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="L33" s="8" t="s">
+      <c r="N33" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="O33" s="6" t="s">
         <v>316</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="T33" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="U33" s="6" t="s">
         <v>37</v>
       </c>
       <c r="V33" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="W33" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4563,58 +4563,58 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="H34" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="K34" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="G34" s="6" t="s">
+      <c r="L34" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="K34" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>324</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W34" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4622,58 +4622,58 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="H35" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="K35" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="L35" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q35" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4681,55 +4681,55 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D36" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="K36" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="F36" s="6" t="s">
+      <c r="L36" s="8" t="s">
         <v>340</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>342</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P36" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="X36" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4737,61 +4737,61 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D37" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="K37" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="G37" s="6" t="s">
+      <c r="L37" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>350</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="X37" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4799,43 +4799,43 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="G38" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="G38" s="6" t="s">
+      <c r="I38" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="K38" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="L38" s="13" t="s">
         <v>359</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>361</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>35</v>
@@ -4844,19 +4844,19 @@
         <v>57</v>
       </c>
       <c r="S38" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="T38" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="U38" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="V38" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="W38" s="6" t="s">
         <v>364</v>
-      </c>
-      <c r="T38" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="U38" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="V38" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="W38" s="6" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4864,55 +4864,55 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="G39" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="F39" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="K39" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="L39" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="M39" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N39" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="O39" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="M39" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>374</v>
-      </c>
       <c r="P39" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="V39" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4920,58 +4920,58 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D40" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="F40" s="6" t="s">
+      <c r="K40" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="L40" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="M40" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N40" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="O40" s="6" t="s">
         <v>380</v>
-      </c>
-      <c r="M40" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="O40" s="6" t="s">
-        <v>382</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q40" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S40" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="T40" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="V40" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W40" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="X40" s="6" t="s">
         <v>383</v>
-      </c>
-      <c r="T40" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="V40" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W40" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="X40" s="6" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4979,58 +4979,58 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="K41" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="G41" s="6" t="s">
+      <c r="L41" s="8" t="s">
         <v>388</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="M41" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q41" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="V41" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="W41" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X41" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5038,55 +5038,55 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="K42" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="L42" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="P42" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q42" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="U42" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="V42" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5094,55 +5094,55 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="L43" s="8" t="s">
         <v>403</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>405</v>
       </c>
       <c r="M43" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="V43" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X43" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5150,55 +5150,55 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N44" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="L44" s="8" t="s">
+      <c r="O44" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="M44" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>413</v>
-      </c>
       <c r="P44" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="U44" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="V44" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X44" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5206,55 +5206,55 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="L45" s="8" t="s">
         <v>415</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>417</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5262,52 +5262,52 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C46" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="K46" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="L46" s="8" t="s">
         <v>425</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>427</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N46" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S46" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="O46" s="6" t="s">
+      <c r="T46" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="P46" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S46" s="6" t="s">
+      <c r="V46" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="T46" s="6" t="s">
+      <c r="W46" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="V46" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="W46" s="6" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5315,49 +5315,49 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="K47" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="L47" s="14" t="s">
         <v>437</v>
-      </c>
-      <c r="K47" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="L47" s="14" t="s">
-        <v>439</v>
       </c>
       <c r="M47" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N47" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S47" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="O47" s="6" t="s">
+      <c r="V47" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="W47" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="P47" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S47" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="V47" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="W47" s="6" t="s">
-        <v>443</v>
-      </c>
       <c r="X47" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5365,55 +5365,55 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="G48" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="K48" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="L48" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="K48" s="7" t="s">
+      <c r="M48" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N48" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="L48" s="8" t="s">
+      <c r="O48" s="6" t="s">
         <v>448</v>
       </c>
-      <c r="M48" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N48" s="6" t="s">
+      <c r="P48" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S48" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="T48" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="O48" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="P48" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S48" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="T48" s="6" t="s">
-        <v>451</v>
-      </c>
       <c r="V48" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5421,55 +5421,55 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="K49" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="L49" s="8" t="s">
         <v>455</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>457</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S49" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="T49" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="V49" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="T49" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="V49" s="6" t="s">
-        <v>432</v>
-      </c>
       <c r="W49" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5477,52 +5477,52 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D50" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="K50" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="L50" s="8" t="s">
         <v>461</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>463</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N50" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="P50" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="S50" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="O50" s="6" t="s">
+      <c r="T50" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="P50" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="S50" s="6" t="s">
+      <c r="V50" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="T50" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="V50" s="6" t="s">
-        <v>468</v>
-      </c>
       <c r="W50" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5530,52 +5530,52 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>470</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="K51" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="L51" s="8" t="s">
         <v>472</v>
-      </c>
-      <c r="K51" s="7" t="s">
-        <v>473</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>474</v>
       </c>
       <c r="M51" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N51" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="S51" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="O51" s="6" t="s">
+      <c r="T51" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="P51" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="S51" s="6" t="s">
+      <c r="V51" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W51" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="T51" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="V51" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W51" s="6" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5583,55 +5583,55 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C52" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="K52" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="L52" s="8" t="s">
         <v>481</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>472</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>483</v>
       </c>
       <c r="M52" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q52" s="6" t="s">
         <v>57</v>
       </c>
       <c r="S52" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="T52" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="V52" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W52" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="T52" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="V52" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W52" s="6" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5639,61 +5639,61 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D53" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="F53" s="6" t="s">
+      <c r="K53" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="H53" s="6" t="s">
+      <c r="L53" s="8" t="s">
         <v>489</v>
-      </c>
-      <c r="K53" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>491</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N53" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="T53" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="O53" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="P53" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="S53" s="6" t="s">
+      <c r="U53" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="V53" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W53" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="T53" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="U53" s="6" t="s">
+      <c r="X53" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="V53" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W53" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="X53" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5701,64 +5701,64 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="H54" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="K54" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="L54" s="8" t="s">
         <v>499</v>
-      </c>
-      <c r="K54" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="L54" s="8" t="s">
-        <v>501</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q54" s="6" t="s">
         <v>35</v>
       </c>
       <c r="R54" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="S54" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="V54" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X54" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5766,58 +5766,58 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="G55" s="6" t="s">
+      <c r="K55" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="L55" s="8" t="s">
         <v>508</v>
-      </c>
-      <c r="K55" s="7" t="s">
-        <v>509</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>510</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N55" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="P55" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="S55" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="T55" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="O55" s="6" t="s">
+      <c r="U55" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="P55" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="T55" s="6" t="s">
+      <c r="V55" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="W55" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="U55" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="V55" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="W55" s="6" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5825,46 +5825,46 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D56" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="L56" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N56" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="K56" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="L56" s="8" t="s">
+      <c r="O56" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="M56" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="N56" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="O56" s="6" t="s">
-        <v>519</v>
-      </c>
       <c r="P56" s="6" t="s">
-        <v>58</v>
+        <v>536</v>
       </c>
       <c r="S56" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5872,55 +5872,55 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C57" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>461</v>
-      </c>
-      <c r="F57" s="6" t="s">
+      <c r="K57" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="L57" s="8" t="s">
         <v>523</v>
-      </c>
-      <c r="K57" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="L57" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N57" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S57" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T57" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="O57" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="P57" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S57" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="T57" s="6" t="s">
-        <v>528</v>
-      </c>
       <c r="U57" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5928,46 +5928,46 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="K58" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L58" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="M58" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="K58" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="L58" s="13" t="s">
+      <c r="N58" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="M58" s="6" t="s">
+      <c r="O58" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="N58" s="6" t="s">
+      <c r="P58" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="S58" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T58" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="O58" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="P58" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S58" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="T58" s="6" t="s">
-        <v>536</v>
-      </c>
       <c r="V58" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -6035,6 +6035,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7A11A7DF961CC428587DE372F9C797B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4479d4a86de7b259c45e5a73c6b02c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7104dee3-b68d-4fc6-af76-78212a7605a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1efb2fb76da6e7bc543ba0de5d23ee76" ns3:_="">
     <xsd:import namespace="7104dee3-b68d-4fc6-af76-78212a7605a5"/>
@@ -6192,15 +6201,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6208,6 +6208,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B767E0B-7018-4DA6-B0B7-DFC282E8DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6221,14 +6229,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update the data according to DNAS Faculty list_20230927
</commit_message>
<xml_diff>
--- a/data_script/dku_knowledge_230504.xlsx
+++ b/data_script/dku_knowledge_230504.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sd540\Desktop\Division Portal\Interdisciplinary-Knowledge-Map-DKU\data_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499F22B-03CC-470F-B2D7-55DD5A291327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B13E14-0285-400B-8659-6759341FF8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="551">
   <si>
     <t>id</t>
   </si>
@@ -179,9 +179,6 @@
     <t>marcus.werner@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Mathematical physics;General relativistic theory;Gravitational waves;astrophysics;Topology;</t>
-  </si>
-  <si>
     <t>ASTRONOMY &amp; ASTROPHYSICS</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>MATH410</t>
   </si>
   <si>
-    <t xml:space="preserve">MATH305; MATH406 ;MATH410;  </t>
-  </si>
-  <si>
     <t>https://sites.google.com/site/shixinxupage/</t>
   </si>
   <si>
@@ -323,9 +317,6 @@
     <t>https://jiulin90.github.io/</t>
   </si>
   <si>
-    <t>Lecturer</t>
-  </si>
-  <si>
     <t>lin.jiu@dukekunshan.edu.cn</t>
   </si>
   <si>
@@ -338,18 +329,12 @@
     <t>Zhenghui Huo</t>
   </si>
   <si>
-    <t>MATH105; MATH202 ;MATH307; MATH308 ;</t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/zhenghui-huo</t>
   </si>
   <si>
     <t>zhenghui.huo@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Complex analysis;Harmonic analysis;Operator theory;Bergman kernal function</t>
-  </si>
-  <si>
     <t>Pure Math</t>
   </si>
   <si>
@@ -458,9 +443,6 @@
     <t>ming.li369@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Speech and language processing;Machine learning;Statistical modeling;Structure health modeling;Multi-model processing;health monitoring</t>
-  </si>
-  <si>
     <t>ARTIFICIAL INTELLIGENCE</t>
   </si>
   <si>
@@ -704,9 +686,6 @@
     <t xml:space="preserve">BIOL201; BIOL212 ;BIOL304;  </t>
   </si>
   <si>
-    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang</t>
-  </si>
-  <si>
     <t>linfeng.huang@dukekunshan.edu.cn</t>
   </si>
   <si>
@@ -782,18 +761,12 @@
     <t>BIOL307</t>
   </si>
   <si>
-    <t xml:space="preserve">BIOL305; BIOL306 ;BIOL307;  </t>
-  </si>
-  <si>
     <t>https://sites.duke.edu/kimlab</t>
   </si>
   <si>
     <t>hm.kim@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Cell and Molecular Biology;Genetics;Microbiology and Biochemistry;DNA damage and repair</t>
-  </si>
-  <si>
     <t>Genetics</t>
   </si>
   <si>
@@ -809,9 +782,6 @@
     <t>jleelab.org</t>
   </si>
   <si>
-    <t xml:space="preserve">joohyun.lee@dukekunshan.edu.cn </t>
-  </si>
-  <si>
     <t>Plant biologist;Epigenetics;Plant physiology;Genetic engineering</t>
   </si>
   <si>
@@ -854,9 +824,6 @@
     <t>BIOL202</t>
   </si>
   <si>
-    <t>BIOL202; BIOL319 ;</t>
-  </si>
-  <si>
     <t>https://eunyukimlab.com/</t>
   </si>
   <si>
@@ -887,9 +854,6 @@
     <t>ferdinand.kappes@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Molecular Genetics;Plant Physiology;Medical Chemistry;Biochemical Pharmacology</t>
-  </si>
-  <si>
     <t>Xianzhi Lin</t>
   </si>
   <si>
@@ -932,21 +896,12 @@
     <t>PHYS405</t>
   </si>
   <si>
-    <t>INTGSCI205; PHYS121 ;PHYS310; PHYS405 ;</t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/kai-huang</t>
   </si>
   <si>
     <t>Associte Professor</t>
   </si>
   <si>
-    <t>Prof Kai Huang, Ph.D. &lt;kai.huang186@duke.edu&gt;</t>
-  </si>
-  <si>
-    <t>Soft matter;Nonequilibrium systems;Phase transition;Collective dynamics;Granular materials;Wetting;Impact mechanics;Particle tracking;Remote sensing (IoTRadar);Digital twin;Room acoustics;human-machine interfact</t>
-  </si>
-  <si>
     <t>PHYSICS, MULTIDISCIPLINARY</t>
   </si>
   <si>
@@ -1160,9 +1115,6 @@
     <t>MATSCI405</t>
   </si>
   <si>
-    <t xml:space="preserve">CHEM401; CHEM402 ;MATSCI405;  </t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/weiwei-shi</t>
   </si>
   <si>
@@ -1208,9 +1160,6 @@
     <t>Mark Spaller</t>
   </si>
   <si>
-    <t>BIOL305; CHEM201 ;</t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/mark-spaller</t>
   </si>
   <si>
@@ -1340,18 +1289,12 @@
     <t>NEUROSCI102</t>
   </si>
   <si>
-    <t xml:space="preserve">BIOL316; NEUROSCI102 ;NEUROSCI301;  </t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/pedro-rada</t>
   </si>
   <si>
     <t>pedro.rada.rincon@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Neuroscience;Behavioral Physiology;Sleep physiology;Brain research;Hydrology;</t>
-  </si>
-  <si>
     <t>NEUROIMAGING</t>
   </si>
   <si>
@@ -1445,18 +1388,12 @@
     <t>Chi-Yeung(Jimmy) Choi</t>
   </si>
   <si>
-    <t>BIOL208; ENVIR102 ;ENVIR315/CHEM315; BIOL318 ；</t>
-  </si>
-  <si>
     <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/chi-yeung-jimmy-choi</t>
   </si>
   <si>
     <t>chiyeung.choi@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Ecology;Global change biology;Landscape ecology;Population biology;Ecosystem ecology;Ornithology;Machine learning;</t>
-  </si>
-  <si>
     <t>ECOLOGY</t>
   </si>
   <si>
@@ -1469,16 +1406,7 @@
     <t>STATS304</t>
   </si>
   <si>
-    <t>BIOL311/ENVIR311; ENVIR208 ;STATS102; STATS304 ;</t>
-  </si>
-  <si>
-    <t>https://sites.duke.edu/sagdku/</t>
-  </si>
-  <si>
     <t>zuchuan.li@dukekunshan.edu.cn</t>
-  </si>
-  <si>
-    <t>Environmental data analysis;Remote sensing;Ocean carbon and oxygen cycling;Ocean physics;Biogeochemistry;Machine learning;Statistics;Statistics</t>
   </si>
   <si>
     <t>REMOTE SENSING</t>
@@ -1695,6 +1623,78 @@
   </si>
   <si>
     <t>Extremophiles; Thermophiles; environmental microbiology; biogeochemistry; bioinformatics</t>
+  </si>
+  <si>
+    <t>BIOL316; NEUROSCI102 ;NEUROSCI301;NEUROSCI 307</t>
+  </si>
+  <si>
+    <t>Neuroscience;Behavioral Physiology;Brain research;</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang; http://www.pro-sirna.com/lab/</t>
+  </si>
+  <si>
+    <t>joohyun.lee@duke.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA damage repair;Histone Epigenetics;Anti-tumor toxicity;Genome Engineering </t>
+  </si>
+  <si>
+    <t>BIOL 212;BIOL305;BIOL306;BIOL307;</t>
+  </si>
+  <si>
+    <t>Molecular Genetics;Medical Chemistry;Biochemical Pharmacology</t>
+  </si>
+  <si>
+    <t>Ornithology; Migration Ecology;Conservation Biology;Global change biology; Remote sensing; Machine learning</t>
+  </si>
+  <si>
+    <t>BIOL208;BIOL318;BIOL322;BIOL406;</t>
+  </si>
+  <si>
+    <t>BIOL202; BIOL319;BIOL 321</t>
+  </si>
+  <si>
+    <t>https://scholars.duke.edu/person/zuchuan.li</t>
+  </si>
+  <si>
+    <t>Machine learning;Bayesian statistics;Environmental data science</t>
+  </si>
+  <si>
+    <t>STATS102;STATS304;ENVIR208</t>
+  </si>
+  <si>
+    <t>BIOL305; CHEM201 ;GLOCHALL 201</t>
+  </si>
+  <si>
+    <t>kai.huang186@duke.edu</t>
+  </si>
+  <si>
+    <t>Soft matter;Nonequilibrium system; Phase transitions; Granular matter; Wetting; Impact mechanics; Radar Particle tracking; Room acoustics; Product Lifecycle Management</t>
+  </si>
+  <si>
+    <t>Environmental science and sustainability &amp; Data and Computer Science</t>
+  </si>
+  <si>
+    <t>INTGSCI205; PHYS121; PHYS122; PHYS310; PHYS405</t>
+  </si>
+  <si>
+    <t>CHEM110; CHEM401; CHEM402; MATSCI401; MATSCI405</t>
+  </si>
+  <si>
+    <t>MATH 203; MATH 305; MATH 406; MATH 410</t>
+  </si>
+  <si>
+    <t>MATH105; MATH307; MATH308 ;</t>
+  </si>
+  <si>
+    <t>Complex analysis; Harmonic analysis; Operator theory;</t>
+  </si>
+  <si>
+    <t>Mathematical physics; General relativistic theory; Gravitational waves; Astrophysics; Differential geometry and topology;</t>
+  </si>
+  <si>
+    <t>Intelligent Speech Processing; Affective Computing; Behavior Signal Processing</t>
   </si>
 </sst>
 </file>
@@ -2697,7 +2697,7 @@
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="N70" sqref="N70"/>
+      <selection pane="bottomLeft" activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2710,11 +2710,11 @@
     <col min="11" max="11" width="70.453125" style="7" customWidth="1"/>
     <col min="12" max="12" width="63.1796875" style="6" customWidth="1"/>
     <col min="13" max="13" width="26" style="6" customWidth="1"/>
-    <col min="14" max="14" width="22.453125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="63.90625" style="6" customWidth="1"/>
     <col min="15" max="15" width="81.08984375" style="6" customWidth="1"/>
     <col min="16" max="16" width="70.54296875" style="6" customWidth="1"/>
-    <col min="17" max="17" width="34.1796875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="10" style="6" customWidth="1"/>
+    <col min="17" max="17" width="62.90625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="43.81640625" style="6" customWidth="1"/>
     <col min="19" max="19" width="49.453125" style="6" customWidth="1"/>
     <col min="20" max="20" width="37.81640625" style="6" customWidth="1"/>
     <col min="21" max="21" width="29.1796875" style="6" customWidth="1"/>
@@ -2886,7 +2886,7 @@
         <v>45</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>46</v>
+        <v>549</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>35</v>
@@ -2895,7 +2895,7 @@
         <v>36</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>38</v>
@@ -2915,46 +2915,46 @@
         <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="K4" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="M4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>36</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V4" s="6" t="s">
         <v>38</v>
@@ -2974,43 +2974,43 @@
         <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="K5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="L5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="M5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="N5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V5" s="6" t="s">
         <v>38</v>
@@ -3030,49 +3030,49 @@
         <v>25</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="6" t="s">
+      <c r="K6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="L6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="M6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="O6" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>36</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="V6" s="6" t="s">
         <v>38</v>
@@ -3092,43 +3092,43 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="K7" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="L7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="M7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="O7" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V7" s="6" t="s">
         <v>38</v>
@@ -3148,49 +3148,49 @@
         <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="L8" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="M8" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="O8" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="V8" s="6" t="s">
         <v>38</v>
@@ -3210,13 +3210,13 @@
         <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>41</v>
@@ -3225,25 +3225,25 @@
         <v>29</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>99</v>
+        <v>547</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>102</v>
+        <v>548</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="V9" s="6" t="s">
         <v>38</v>
@@ -3263,49 +3263,49 @@
         <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="V10" s="6" t="s">
         <v>38</v>
@@ -3325,52 +3325,52 @@
         <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="K11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="L11" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="M11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>38</v>
@@ -3379,7 +3379,7 @@
         <v>24</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3393,46 +3393,46 @@
         <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>28</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V12" s="6" t="s">
         <v>38</v>
@@ -3452,28 +3452,28 @@
         <v>25</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>537</v>
+        <v>513</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>538</v>
+        <v>514</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>540</v>
+        <v>516</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>541</v>
+        <v>517</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>38</v>
@@ -3482,7 +3482,7 @@
         <v>24</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3490,58 +3490,58 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>139</v>
+        <v>550</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R14" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3549,49 +3549,49 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="P15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S15" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="T15" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3599,55 +3599,55 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="O16" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="P16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="S16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="T16" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="U16" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="V16" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3655,61 +3655,61 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="V17" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W17" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3717,64 +3717,64 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="V18" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W18" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3782,61 +3782,61 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D19" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="O19" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="P19" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="V19" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="X19" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3844,61 +3844,61 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="U20" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="V20" s="6" t="s">
         <v>38</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3906,55 +3906,55 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D21" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="P21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="U21" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="P21" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="S21" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="T21" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="U21" s="6" t="s">
-        <v>158</v>
-      </c>
       <c r="V21" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W21" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3962,46 +3962,46 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>523</v>
+        <v>499</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>524</v>
+        <v>500</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>525</v>
+        <v>501</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>526</v>
+        <v>502</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>530</v>
+        <v>506</v>
       </c>
       <c r="V22" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="W22" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:24" s="9" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4009,52 +4009,52 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="L23" s="14" t="s">
         <v>202</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>208</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>32</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="P23" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S23" s="9" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="V23" s="9" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="X23" s="9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4062,55 +4062,55 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>221</v>
+        <v>529</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="V24" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W24" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4118,52 +4118,52 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="T25" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="V25" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="X25" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4171,58 +4171,58 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="O26" s="6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q26" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="U26" s="6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V26" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W26" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="X26" s="6" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4230,52 +4230,52 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>247</v>
+        <v>532</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>250</v>
+        <v>531</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="V27" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W27" s="6" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="X27" s="6" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4283,58 +4283,58 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>256</v>
+        <v>52</v>
+      </c>
+      <c r="N28" s="12" t="s">
+        <v>530</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="U28" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="V28" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="W28" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="V28" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="W28" s="6" t="s">
-        <v>251</v>
-      </c>
       <c r="X28" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4342,64 +4342,64 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="V29" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W29" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="X29" s="6" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4407,55 +4407,55 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>271</v>
+        <v>536</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="O30" s="6" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="V30" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W30" s="6" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4463,55 +4463,55 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>282</v>
+        <v>533</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="U31" s="6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V31" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W31" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="X31" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4519,49 +4519,49 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="V32" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W32" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -4569,47 +4569,47 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>532</v>
+        <v>508</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="6" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="T33" s="16" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="V33" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W33" s="16" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="X33" s="17" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4617,67 +4617,67 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>297</v>
+        <v>544</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>300</v>
+        <v>286</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>541</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>301</v>
+        <v>542</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>240</v>
+        <v>543</v>
       </c>
       <c r="R34" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="U34" s="6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W34" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="X34" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="X34" s="6" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4685,55 +4685,55 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>306</v>
-      </c>
       <c r="E35" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="K35" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>309</v>
-      </c>
       <c r="L35" s="8" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="U35" s="6" t="s">
         <v>37</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4741,58 +4741,58 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K36" s="7" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="P36" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q36" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4800,58 +4800,58 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4859,55 +4859,55 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="V38" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W38" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="X38" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="X38" s="6" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4915,61 +4915,61 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q39" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="V39" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4977,55 +4977,55 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S40" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="V40" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5033,58 +5033,58 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="L41" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="E41" s="6" t="s">
+      <c r="M41" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="O41" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q41" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="V41" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W41" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="X41" s="6" t="s">
-        <v>369</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5092,58 +5092,58 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>373</v>
+        <v>545</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q42" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="T42" s="6" t="s">
-        <v>368</v>
+        <v>353</v>
       </c>
       <c r="V42" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>378</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5151,55 +5151,55 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="U43" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="V43" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5207,55 +5207,55 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>389</v>
+        <v>540</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="P44" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>367</v>
+        <v>352</v>
       </c>
       <c r="V44" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="X44" s="6" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5263,55 +5263,55 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5319,55 +5319,55 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="U46" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="W46" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="X46" s="6" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5375,52 +5375,52 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="T47" s="6" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="V47" s="6" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="W47" s="6" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5428,49 +5428,49 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C48" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="K48" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>424</v>
-      </c>
       <c r="L48" s="13" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="M48" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="P48" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="V48" s="6" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5478,55 +5478,55 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>433</v>
+        <v>527</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>436</v>
+        <v>528</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5534,55 +5534,55 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>439</v>
-      </c>
       <c r="F50" s="6" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>445</v>
+        <v>426</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S50" s="6" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="T50" s="6" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="V50" s="6" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="W50" s="6" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5590,161 +5590,164 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>446</v>
+        <v>427</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>449</v>
+        <v>430</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="P51" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S51" s="6" t="s">
-        <v>452</v>
+        <v>433</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="V51" s="6" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="W51" s="6" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="K52" s="7" t="s">
-        <v>459</v>
+        <v>440</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>460</v>
+        <v>441</v>
       </c>
       <c r="M52" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S52" s="6" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>464</v>
+        <v>445</v>
       </c>
       <c r="V52" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W52" s="6" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>456</v>
+        <v>437</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>458</v>
+        <v>439</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>468</v>
+        <v>535</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>471</v>
+        <v>534</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q53" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S53" s="6" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="V53" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>465</v>
+        <v>446</v>
+      </c>
+      <c r="X53" s="6" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5752,61 +5755,64 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>476</v>
+        <v>539</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>477</v>
+        <v>537</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>479</v>
+        <v>538</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="S54" s="6" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="U54" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V54" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>465</v>
+        <v>234</v>
       </c>
       <c r="X54" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5814,64 +5820,64 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>489</v>
+        <v>465</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Q55" s="6" t="s">
         <v>35</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="S55" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
       <c r="V55" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W55" s="6" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="X55" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5879,58 +5885,58 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>493</v>
+        <v>469</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>494</v>
+        <v>470</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>495</v>
+        <v>471</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>496</v>
+        <v>472</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>497</v>
+        <v>473</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>498</v>
+        <v>474</v>
       </c>
       <c r="P56" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S56" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>499</v>
+        <v>475</v>
       </c>
       <c r="U56" s="6" t="s">
-        <v>500</v>
+        <v>476</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>501</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5938,46 +5944,46 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>550</v>
+        <v>526</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="S57" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="U57" s="6" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5985,46 +5991,46 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>466</v>
+        <v>447</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="O58" s="6" t="s">
-        <v>505</v>
+        <v>481</v>
       </c>
       <c r="P58" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S58" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
       <c r="V58" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6032,55 +6038,55 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>506</v>
+        <v>482</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>507</v>
+        <v>483</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>447</v>
+        <v>428</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S59" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="U59" s="6" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="W59" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6088,46 +6094,46 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>506</v>
+        <v>482</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>516</v>
+        <v>492</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="K60" s="7" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="L60" s="12" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>520</v>
+        <v>496</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>521</v>
+        <v>497</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S60" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>522</v>
+        <v>498</v>
       </c>
       <c r="V60" s="6" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="W60" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -6144,7 +6150,7 @@
     <hyperlink ref="L16" r:id="rId10" xr:uid="{273DF806-1BFB-4885-AAA0-2A07D17AEDC1}"/>
     <hyperlink ref="L17" r:id="rId11" xr:uid="{4BB0B568-E23C-4D60-BB58-2B6921573820}"/>
     <hyperlink ref="L19" r:id="rId12" xr:uid="{7977FBFE-C6C2-44B0-A7F6-04A06D6F7F49}"/>
-    <hyperlink ref="L24" r:id="rId13" xr:uid="{69D3DB11-C5D2-4F29-B8E7-9D93439B647A}"/>
+    <hyperlink ref="L24" r:id="rId13" display="https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang" xr:uid="{69D3DB11-C5D2-4F29-B8E7-9D93439B647A}"/>
     <hyperlink ref="L25" r:id="rId14" xr:uid="{00A85A45-8229-4A7C-A09E-056A341C953E}"/>
     <hyperlink ref="L26" r:id="rId15" xr:uid="{F6A8F67C-D69D-407F-9920-2F13D7D2912D}"/>
     <hyperlink ref="L29" r:id="rId16" xr:uid="{523EB51B-334C-4C4D-89C5-0A1D06556799}"/>
@@ -6187,13 +6193,24 @@
     <hyperlink ref="L39" r:id="rId53" xr:uid="{1FCD329E-6B84-4EAA-B176-7B053A3DA255}"/>
     <hyperlink ref="L48" r:id="rId54" xr:uid="{4C9656AE-E61B-4DFE-B3E7-7A985DB1D5D6}"/>
     <hyperlink ref="L22" r:id="rId55" xr:uid="{5D37EC19-4EB9-4DD8-9B95-EA7F0EB869CB}"/>
+    <hyperlink ref="N28" r:id="rId56" xr:uid="{DFB81A75-9D40-4E3C-AB20-DA2B413EE03E}"/>
+    <hyperlink ref="N34" r:id="rId57" xr:uid="{C7C9B0B7-320E-4598-BE11-8BB3E848B2B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7A11A7DF961CC428587DE372F9C797B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4479d4a86de7b259c45e5a73c6b02c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7104dee3-b68d-4fc6-af76-78212a7605a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1efb2fb76da6e7bc543ba0de5d23ee76" ns3:_="">
     <xsd:import namespace="7104dee3-b68d-4fc6-af76-78212a7605a5"/>
@@ -6351,15 +6368,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6367,6 +6375,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B767E0B-7018-4DA6-B0B7-DFC282E8DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6384,14 +6400,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
move the close button in hint box to right-top; update the information of bingluo
</commit_message>
<xml_diff>
--- a/data_script/dku_knowledge_230504.xlsx
+++ b/data_script/dku_knowledge_230504.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sd540\Desktop\Division Portal\Interdisciplinary-Knowledge-Map-DKU\data_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B13E14-0285-400B-8659-6759341FF8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D02D99E-06C0-4523-BBB9-B1BADA1F17F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dku_knowledge_230216" sheetId="1" r:id="rId1"/>
@@ -623,9 +623,6 @@
     <t>bing.luo@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Edge learning;Networking;Game Theory;Optimization;embedded AI;IoT</t>
-  </si>
-  <si>
     <t>Biology</t>
   </si>
   <si>
@@ -1035,9 +1032,6 @@
   </si>
   <si>
     <t>domna.kotsifaki@dukekunshan.edu.cn</t>
-  </si>
-  <si>
-    <t>Biophysics;Nano-photonics;Optical tweezer;Plasmonics;Metamaterials;Sensing;Optical tweezers;</t>
   </si>
   <si>
     <t>BIOPHYSICS</t>
@@ -1551,9 +1545,6 @@
     <t>kaizhu.huang@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Machine Learning, Pattern Recognition, Computer Vision</t>
-  </si>
-  <si>
     <t>Artificial Intelligence</t>
   </si>
   <si>
@@ -1695,6 +1686,15 @@
   </si>
   <si>
     <t>Intelligent Speech Processing; Affective Computing; Behavior Signal Processing</t>
+  </si>
+  <si>
+    <t>Biophysics;Nano-photonics;Optical tweezer;Plasmonics;Metamaterials;Sensing;</t>
+  </si>
+  <si>
+    <t>Machine Learning; Pattern Recognition; Computer Vision</t>
+  </si>
+  <si>
+    <t>Edge Computing; Machine Learning; Wireless Communications; Networking; Game Theory; Optimization; IoT</t>
   </si>
 </sst>
 </file>
@@ -2694,37 +2694,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L70" sqref="L70"/>
+      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" style="6" customWidth="1"/>
-    <col min="5" max="10" width="12.81640625" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="70.453125" style="7" customWidth="1"/>
-    <col min="12" max="12" width="63.1796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
+    <col min="5" max="10" width="12.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="70.42578125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="63.140625" style="6" customWidth="1"/>
     <col min="13" max="13" width="26" style="6" customWidth="1"/>
-    <col min="14" max="14" width="63.90625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="81.08984375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="70.54296875" style="6" customWidth="1"/>
-    <col min="17" max="17" width="62.90625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="43.81640625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="49.453125" style="6" customWidth="1"/>
-    <col min="20" max="20" width="37.81640625" style="6" customWidth="1"/>
-    <col min="21" max="21" width="29.1796875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="49.1796875" style="6" customWidth="1"/>
-    <col min="23" max="23" width="28.1796875" style="6" customWidth="1"/>
-    <col min="24" max="24" width="29.54296875" style="6" customWidth="1"/>
-    <col min="25" max="16384" width="8.81640625" style="6"/>
+    <col min="14" max="14" width="63.85546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="81.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="70.5703125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="62.85546875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="43.85546875" style="6" customWidth="1"/>
+    <col min="19" max="19" width="49.42578125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="37.85546875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="29.140625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="49.140625" style="6" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" style="6" customWidth="1"/>
+    <col min="24" max="24" width="29.5703125" style="6" customWidth="1"/>
+    <col min="25" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>45</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>35</v>
@@ -2904,7 +2904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>50</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>51</v>
@@ -2963,7 +2963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>29</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>96</v>
@@ -3237,7 +3237,7 @@
         <v>97</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>35</v>
@@ -3252,7 +3252,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:24" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:24" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3452,28 +3452,28 @@
         <v>25</v>
       </c>
       <c r="D13" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>513</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="N13" s="6" t="s">
         <v>514</v>
       </c>
-      <c r="L13" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>517</v>
-      </c>
       <c r="O13" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>38</v>
@@ -3482,10 +3482,10 @@
         <v>24</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>133</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>55</v>
@@ -3544,7 +3544,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>193</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>194</v>
+        <v>550</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>55</v>
@@ -3957,7 +3957,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -3968,34 +3968,34 @@
         <v>127</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>111</v>
       </c>
       <c r="L22" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="N22" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>502</v>
-      </c>
       <c r="O22" s="6" t="s">
-        <v>503</v>
+        <v>549</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>55</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="V22" s="6" t="s">
         <v>136</v>
@@ -4004,777 +4004,777 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" s="9" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="K23" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="L23" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>202</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>32</v>
       </c>
       <c r="N23" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="O23" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="O23" s="9" t="s">
-        <v>204</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>56</v>
       </c>
       <c r="S23" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="V23" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="V23" s="9" t="s">
+      <c r="W23" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="W23" s="9" t="s">
+      <c r="X23" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="X23" s="9" t="s">
-        <v>208</v>
-      </c>
     </row>
-    <row r="24" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D24" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="K24" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="K24" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="L24" s="8" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N24" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="O24" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="O24" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S24" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="V24" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="V24" s="6" t="s">
+      <c r="W24" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="W24" s="6" t="s">
+      <c r="X24" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="X24" s="6" t="s">
-        <v>208</v>
-      </c>
     </row>
-    <row r="25" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D25" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="K25" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="L25" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="M25" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="N25" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="N25" s="6" t="s">
+      <c r="O25" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S25" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="V25" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="T25" s="6" t="s">
+      <c r="W25" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="X25" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="V25" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>225</v>
-      </c>
     </row>
-    <row r="26" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D26" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="K26" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="L26" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N26" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O26" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="O26" s="6" t="s">
+      <c r="P26" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S26" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="U26" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="U26" s="6" t="s">
+      <c r="V26" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="W26" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="X26" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="V26" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W26" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="X26" s="6" t="s">
-        <v>236</v>
-      </c>
     </row>
-    <row r="27" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D27" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="K27" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="L27" s="12" t="s">
         <v>239</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="L27" s="12" t="s">
-        <v>240</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S27" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="V27" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="V27" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="W27" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X27" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D28" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="K28" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="L28" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>246</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>56</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S28" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T28" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="U28" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="V28" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="T28" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="U28" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="V28" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="W28" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X28" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D29" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="K29" s="7" t="s">
+      <c r="L29" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>255</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N29" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="O29" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="O29" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="P29" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V29" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W29" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="X29" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D30" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="L30" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="L30" s="12" t="s">
+      <c r="M30" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="N30" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>56</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S30" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T30" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="V30" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="T30" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="V30" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="W30" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D31" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="G31" s="6" t="s">
+      <c r="K31" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="L31" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="M31" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="N31" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="N31" s="6" t="s">
-        <v>270</v>
-      </c>
       <c r="O31" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S31" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="U31" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="V31" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="U31" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="V31" s="6" t="s">
+      <c r="W31" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="W31" s="6" t="s">
+      <c r="X31" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="X31" s="6" t="s">
-        <v>208</v>
-      </c>
     </row>
-    <row r="32" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D32" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="F32" s="6" t="s">
+      <c r="K32" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="L32" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>274</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>192</v>
       </c>
       <c r="N32" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="O32" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="O32" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="P32" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S32" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="V32" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="V32" s="6" t="s">
+      <c r="W32" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="W32" s="6" t="s">
-        <v>207</v>
-      </c>
       <c r="X32" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:24" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="D33" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="L33" s="8"/>
       <c r="M33" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S33" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="T33" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="U33" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="V33" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="T33" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="U33" s="6" t="s">
-        <v>507</v>
-      </c>
-      <c r="V33" s="6" t="s">
-        <v>206</v>
-      </c>
       <c r="W33" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X33" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="K34" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="K34" s="7" t="s">
-        <v>544</v>
-      </c>
-      <c r="L34" s="8" t="s">
+      <c r="M34" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>286</v>
-      </c>
       <c r="N34" s="12" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>55</v>
       </c>
       <c r="S34" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="T34" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="T34" s="6" t="s">
+      <c r="U34" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="V34" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="U34" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="V34" s="6" t="s">
+      <c r="W34" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="X34" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="W34" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="X34" s="6" t="s">
-        <v>290</v>
-      </c>
     </row>
-    <row r="35" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D35" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="K35" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="L35" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="M35" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="N35" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="N35" s="6" t="s">
+      <c r="O35" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U35" s="6" t="s">
         <v>37</v>
       </c>
       <c r="V35" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D36" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="F36" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="H36" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="K36" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="K36" s="7" t="s">
+      <c r="L36" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N36" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="O36" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="O36" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="P36" s="6" t="s">
         <v>35</v>
@@ -4783,172 +4783,172 @@
         <v>56</v>
       </c>
       <c r="S36" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="T36" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="T36" s="6" t="s">
-        <v>308</v>
-      </c>
       <c r="V36" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D37" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="H37" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="K37" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="K37" s="7" t="s">
+      <c r="L37" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>314</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N37" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="O37" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q37" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S37" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="T37" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="T37" s="6" t="s">
-        <v>318</v>
-      </c>
       <c r="V37" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D38" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="F38" s="6" t="s">
+      <c r="G38" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="K38" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="K38" s="7" t="s">
+      <c r="L38" s="8" t="s">
         <v>321</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N38" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="O38" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="O38" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S38" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="T38" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="T38" s="6" t="s">
-        <v>326</v>
-      </c>
       <c r="V38" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="W38" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="X38" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="W38" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="X38" s="6" t="s">
-        <v>290</v>
-      </c>
     </row>
-    <row r="39" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D39" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="G39" s="6" t="s">
+      <c r="H39" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="K39" s="7" t="s">
+      <c r="L39" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>330</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>332</v>
+        <v>548</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>35</v>
@@ -4957,113 +4957,113 @@
         <v>56</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="V39" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="K40" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="L40" s="8" t="s">
         <v>339</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>341</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>149</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S40" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="V40" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="F41" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="F41" s="6" t="s">
+      <c r="K41" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="L41" s="8" t="s">
         <v>347</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>349</v>
       </c>
       <c r="M41" s="6" t="s">
         <v>149</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>35</v>
@@ -5072,169 +5072,169 @@
         <v>56</v>
       </c>
       <c r="S41" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="T41" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="V41" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="W41" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="X41" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="T41" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="V41" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W41" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="X41" s="6" t="s">
-        <v>354</v>
-      </c>
     </row>
-    <row r="42" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="K42" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="L42" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>358</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q42" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S42" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="T42" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="V42" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="S42" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="T42" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="V42" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="W42" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="F43" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="F43" s="6" t="s">
+      <c r="K43" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="L43" s="8" t="s">
         <v>365</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>367</v>
       </c>
       <c r="M43" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="U43" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="V43" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="P44" s="6" t="s">
         <v>56</v>
@@ -5243,897 +5243,897 @@
         <v>35</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="T44" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="V44" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="X44" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="L45" s="8" t="s">
         <v>378</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>149</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="L46" s="8" t="s">
         <v>384</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>386</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="U46" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="W46" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="X46" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C47" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="G47" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="K47" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="L47" s="8" t="s">
         <v>394</v>
-      </c>
-      <c r="K47" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>396</v>
       </c>
       <c r="M47" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="P47" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S47" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="T47" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="V47" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="T47" s="6" t="s">
+      <c r="W47" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="V47" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="W47" s="6" t="s">
-        <v>402</v>
-      </c>
     </row>
-    <row r="48" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="K48" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="L48" s="13" t="s">
         <v>406</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="L48" s="13" t="s">
-        <v>408</v>
       </c>
       <c r="M48" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="V48" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="X48" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="G49" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="L49" s="8" t="s">
         <v>414</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>527</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>416</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>64</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="X49" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D50" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="G50" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="K50" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="L50" s="8" t="s">
         <v>422</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>423</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>424</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P50" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S50" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="T50" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="V50" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="T50" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="V50" s="6" t="s">
-        <v>401</v>
-      </c>
       <c r="W50" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D51" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="K51" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="L51" s="8" t="s">
         <v>428</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="K51" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>430</v>
       </c>
       <c r="M51" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N51" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S51" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="O51" s="6" t="s">
+      <c r="T51" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="P51" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="S51" s="6" t="s">
+      <c r="V51" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="T51" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="V51" s="6" t="s">
-        <v>435</v>
-      </c>
       <c r="W51" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="X51" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D52" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="G52" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="K52" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="L52" s="8" t="s">
         <v>439</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>440</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>441</v>
       </c>
       <c r="M52" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N52" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S52" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="O52" s="6" t="s">
+      <c r="T52" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="P52" s="6" t="s">
+      <c r="V52" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="S52" s="6" t="s">
+      <c r="W52" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="T52" s="6" t="s">
-        <v>445</v>
-      </c>
-      <c r="V52" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W52" s="6" t="s">
-        <v>446</v>
-      </c>
     </row>
-    <row r="53" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C53" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="L53" s="8" t="s">
         <v>447</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>439</v>
-      </c>
-      <c r="K53" s="7" t="s">
-        <v>535</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>449</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="P53" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q53" s="6" t="s">
         <v>55</v>
       </c>
       <c r="S53" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="V53" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="W53" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="T53" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="V53" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W53" s="6" t="s">
-        <v>446</v>
-      </c>
       <c r="X53" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>130</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q54" s="6" t="s">
         <v>136</v>
       </c>
       <c r="S54" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="U54" s="6" t="s">
         <v>118</v>
       </c>
       <c r="V54" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="X54" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="H55" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="K55" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="L55" s="8" t="s">
         <v>461</v>
-      </c>
-      <c r="K55" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>463</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q55" s="6" t="s">
         <v>35</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="S55" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="T55" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="V55" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W55" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="X55" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D56" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="G56" s="6" t="s">
+      <c r="K56" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="L56" s="8" t="s">
         <v>470</v>
-      </c>
-      <c r="K56" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="L56" s="8" t="s">
-        <v>472</v>
       </c>
       <c r="M56" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N56" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="T56" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="O56" s="6" t="s">
+      <c r="U56" s="6" t="s">
         <v>474</v>
       </c>
-      <c r="P56" s="6" t="s">
+      <c r="V56" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="S56" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="T56" s="6" t="s">
+      <c r="W56" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="U56" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="V56" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="W56" s="6" t="s">
-        <v>477</v>
-      </c>
     </row>
-    <row r="57" spans="1:24" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="L57" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="M57" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="K57" s="7" t="s">
+      <c r="N57" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="L57" s="8" t="s">
+      <c r="O57" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="M57" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="N57" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="O57" s="6" t="s">
-        <v>526</v>
-      </c>
       <c r="P57" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S57" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="U57" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
-    <row r="58" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="M58" s="6" t="s">
         <v>149</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O58" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S58" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="V58" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
-    <row r="59" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C59" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F59" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="G59" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="F59" s="6" t="s">
+      <c r="K59" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="L59" s="8" t="s">
         <v>485</v>
-      </c>
-      <c r="K59" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="L59" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="M59" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S59" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="U59" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="W59" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="K60" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="L60" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="M60" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="K60" s="7" t="s">
-        <v>493</v>
-      </c>
-      <c r="L60" s="12" t="s">
+      <c r="N60" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="M60" s="6" t="s">
+      <c r="O60" s="6" t="s">
         <v>495</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="O60" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S60" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T60" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="V60" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="W60" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -6202,15 +6202,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7A11A7DF961CC428587DE372F9C797B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4479d4a86de7b259c45e5a73c6b02c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7104dee3-b68d-4fc6-af76-78212a7605a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1efb2fb76da6e7bc543ba0de5d23ee76" ns3:_="">
     <xsd:import namespace="7104dee3-b68d-4fc6-af76-78212a7605a5"/>
@@ -6368,21 +6359,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B767E0B-7018-4DA6-B0B7-DFC282E8DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6400,11 +6392,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix badlinks of faculty page and modify addcording to professors
</commit_message>
<xml_diff>
--- a/data_script/dku_knowledge_230504.xlsx
+++ b/data_script/dku_knowledge_230504.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sd540\Desktop\Division Portal\Interdisciplinary-Knowledge-Map-DKU\data_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D02D99E-06C0-4523-BBB9-B1BADA1F17F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60345FB1-A667-45B9-AFA1-4223F89F5D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="dku_knowledge_230216" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dku_knowledge_230216!$A$1:$X$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dku_knowledge_230216!$A$1:$X$59</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="544">
   <si>
     <t>id</t>
   </si>
@@ -776,9 +776,6 @@
     <t>BIOL110; BIOL315 ;</t>
   </si>
   <si>
-    <t>jleelab.org</t>
-  </si>
-  <si>
     <t>Plant biologist;Epigenetics;Plant physiology;Genetic engineering</t>
   </si>
   <si>
@@ -803,9 +800,6 @@
     <t>BIOL311/ENVIR311; BIOL314 ;BIOL317; ENVIR202 ;</t>
   </si>
   <si>
-    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/cao-huansheng/</t>
-  </si>
-  <si>
     <t>huansheng.cao@dukekunshan.edu.cn</t>
   </si>
   <si>
@@ -1040,33 +1034,9 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>Song Gao</t>
-  </si>
-  <si>
     <t>CHEM110</t>
   </si>
   <si>
-    <t>CHEM150</t>
-  </si>
-  <si>
-    <t>ENVIR304</t>
-  </si>
-  <si>
-    <t>ENVIR402</t>
-  </si>
-  <si>
-    <t>CHEM110; CHEM150 ;ENVIR304; ENVIR402 ;</t>
-  </si>
-  <si>
-    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/song-gao</t>
-  </si>
-  <si>
-    <t>song.gao212@dukekunshan.edu.cn</t>
-  </si>
-  <si>
-    <t>Atmospheric chemistry;Aerosol dynamics (mechanisms characterization)Analytical chemistry;Density functional theory;Climate mitigation;Climate pollutants;Air pollution;Water pollution;</t>
-  </si>
-  <si>
     <t>Environmental Science</t>
   </si>
   <si>
@@ -1506,9 +1476,6 @@
   </si>
   <si>
     <t>VIROLOGY</t>
-  </si>
-  <si>
-    <t>Global Health - Biological Sciences</t>
   </si>
   <si>
     <t>Sajid Umar</t>
@@ -1589,12 +1556,6 @@
     <t>cristiano.villa@dukekunshan.edu.cn</t>
   </si>
   <si>
-    <t>Cristiano Villa | Scholars@Duke profile</t>
-  </si>
-  <si>
-    <t>Statistics and Probability</t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -1622,9 +1583,6 @@
     <t>Neuroscience;Behavioral Physiology;Brain research;</t>
   </si>
   <si>
-    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang; http://www.pro-sirna.com/lab/</t>
-  </si>
-  <si>
     <t>joohyun.lee@duke.edu</t>
   </si>
   <si>
@@ -1695,6 +1653,27 @@
   </si>
   <si>
     <t>Edge Computing; Machine Learning; Wireless Communications; Networking; Game Theory; Optimization; IoT</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/huansheng-cao</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/joohyun-lee</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/cristiano-villa</t>
+  </si>
+  <si>
+    <t>Global Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://scholars.duke.edu/person/Xiangdong.Gao </t>
+  </si>
+  <si>
+    <t>Materials Science</t>
   </si>
 </sst>
 </file>
@@ -2396,9 +2375,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2436,7 +2415,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2542,7 +2521,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2684,7 +2663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2692,18 +2671,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X60"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
+      <selection pane="bottomLeft" activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
     <col min="5" max="10" width="12.85546875" style="6" hidden="1" customWidth="1"/>
@@ -2886,7 +2865,7 @@
         <v>45</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>35</v>
@@ -2927,7 +2906,7 @@
         <v>50</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>51</v>
@@ -3225,7 +3204,7 @@
         <v>29</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>96</v>
@@ -3237,7 +3216,7 @@
         <v>97</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>35</v>
@@ -3452,28 +3431,28 @@
         <v>25</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>515</v>
+        <v>540</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>516</v>
+        <v>67</v>
       </c>
       <c r="V13" s="6" t="s">
         <v>38</v>
@@ -3482,7 +3461,7 @@
         <v>24</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -3517,7 +3496,7 @@
         <v>133</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>55</v>
@@ -3933,7 +3912,7 @@
         <v>193</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>55</v>
@@ -3968,34 +3947,34 @@
         <v>127</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>111</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>55</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="V22" s="6" t="s">
         <v>136</v>
@@ -4086,7 +4065,7 @@
         <v>213</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>526</v>
+        <v>539</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>32</v>
@@ -4248,7 +4227,7 @@
         <v>238</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>239</v>
@@ -4260,7 +4239,7 @@
         <v>240</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>56</v>
@@ -4300,17 +4279,17 @@
       <c r="K28" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>245</v>
+      <c r="L28" s="12" t="s">
+        <v>538</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>56</v>
@@ -4322,7 +4301,7 @@
         <v>204</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U28" s="6" t="s">
         <v>234</v>
@@ -4348,37 +4327,37 @@
         <v>195</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="I29" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="K29" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>253</v>
-      </c>
       <c r="L29" s="8" t="s">
-        <v>254</v>
+        <v>537</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="P29" s="6" t="s">
         <v>232</v>
@@ -4390,7 +4369,7 @@
         <v>204</v>
       </c>
       <c r="T29" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="V29" s="6" t="s">
         <v>233</v>
@@ -4413,28 +4392,28 @@
         <v>195</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>227</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="L30" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="N30" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="O30" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="O30" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="P30" s="6" t="s">
         <v>56</v>
@@ -4446,7 +4425,7 @@
         <v>204</v>
       </c>
       <c r="T30" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="V30" s="6" t="s">
         <v>205</v>
@@ -4469,7 +4448,7 @@
         <v>195</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>197</v>
@@ -4478,22 +4457,22 @@
         <v>209</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="L31" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="M31" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="N31" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>269</v>
-      </c>
       <c r="O31" s="6" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>56</v>
@@ -4525,28 +4504,28 @@
         <v>195</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>243</v>
       </c>
       <c r="F32" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="L32" s="8" t="s">
         <v>271</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>192</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P32" s="6" t="s">
         <v>56</v>
@@ -4561,7 +4540,7 @@
         <v>206</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4575,20 +4554,22 @@
         <v>195</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="L33" s="8"/>
+        <v>495</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>542</v>
+      </c>
       <c r="M33" s="6" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>56</v>
@@ -4600,7 +4581,7 @@
         <v>241</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="V33" s="6" t="s">
         <v>205</v>
@@ -4617,67 +4598,67 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="K34" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="M34" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="K34" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="M34" s="6" t="s">
-        <v>285</v>
-      </c>
       <c r="N34" s="12" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>55</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="T34" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="U34" s="6" t="s">
         <v>234</v>
       </c>
       <c r="V34" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W34" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="X34" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4685,37 +4666,37 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="F35" s="6" t="s">
+      <c r="K35" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="L35" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="M35" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="L35" s="8" t="s">
+      <c r="N35" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="O35" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>35</v>
@@ -4724,7 +4705,7 @@
         <v>234</v>
       </c>
       <c r="T35" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="U35" s="6" t="s">
         <v>37</v>
@@ -4733,7 +4714,7 @@
         <v>205</v>
       </c>
       <c r="W35" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4741,40 +4722,40 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D36" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="H36" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="K36" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="G36" s="6" t="s">
+      <c r="L36" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="P36" s="6" t="s">
         <v>35</v>
@@ -4783,16 +4764,16 @@
         <v>56</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="T36" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V36" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4800,40 +4781,40 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D37" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="G37" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="H37" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="K37" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="L37" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>313</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>35</v>
@@ -4842,16 +4823,16 @@
         <v>232</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="T37" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V37" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W37" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4859,55 +4840,55 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K38" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="F38" s="6" t="s">
+      <c r="L38" s="8" t="s">
         <v>319</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="V38" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W38" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="X38" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4915,40 +4896,40 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="G39" s="6" t="s">
+      <c r="L39" s="12" t="s">
         <v>327</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="L39" s="12" t="s">
-        <v>329</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>35</v>
@@ -4957,337 +4938,337 @@
         <v>56</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V39" s="6" t="s">
         <v>205</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="X39" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>333</v>
       </c>
       <c r="E40" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="K40" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="L40" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>339</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>149</v>
       </c>
       <c r="N40" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="P40" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S40" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="O40" s="6" t="s">
+      <c r="T40" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="P40" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S40" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="V40" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
+      </c>
+      <c r="X40" s="6" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>332</v>
+        <v>543</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>343</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>345</v>
       </c>
       <c r="K41" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="L41" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="M41" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N41" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="M41" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N41" s="6" t="s">
+      <c r="O41" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>349</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>35</v>
       </c>
       <c r="Q41" s="6" t="s">
-        <v>56</v>
+        <v>232</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W41" s="6" t="s">
-        <v>332</v>
+        <v>286</v>
       </c>
       <c r="X41" s="6" t="s">
-        <v>352</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="K42" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="G42" s="6" t="s">
+      <c r="L42" s="8" t="s">
         <v>355</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>356</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N42" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="O42" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="O42" s="6" t="s">
+      <c r="P42" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S42" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="P42" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q42" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="S42" s="6" t="s">
+      <c r="U42" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="T42" s="6" t="s">
-        <v>351</v>
-      </c>
       <c r="V42" s="6" t="s">
-        <v>233</v>
+        <v>286</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="X42" s="6" t="s">
-        <v>233</v>
+        <v>330</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="L43" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="F43" s="6" t="s">
+      <c r="M43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="O43" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="K43" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>367</v>
-      </c>
       <c r="P43" s="6" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="U43" s="6" t="s">
-        <v>369</v>
+        <v>364</v>
+      </c>
+      <c r="T43" s="6" t="s">
+        <v>340</v>
       </c>
       <c r="V43" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
+      </c>
+      <c r="X43" s="6" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="O44" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>537</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="M44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>373</v>
-      </c>
       <c r="P44" s="6" t="s">
-        <v>56</v>
+        <v>232</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="T44" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="U44" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="V44" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="W44" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X44" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="V44" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="W44" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="X44" s="6" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="O45" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="O45" s="6" t="s">
-        <v>380</v>
       </c>
       <c r="P45" s="6" t="s">
         <v>232</v>
@@ -5296,39 +5277,45 @@
         <v>35</v>
       </c>
       <c r="S45" s="6" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="T45" s="6" t="s">
-        <v>306</v>
+        <v>377</v>
       </c>
       <c r="U45" s="6" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="V45" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>332</v>
+        <v>391</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>278</v>
+        <v>378</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="G46" s="6" t="s">
         <v>382</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>383</v>
@@ -5337,7 +5324,7 @@
         <v>384</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="N46" s="6" t="s">
         <v>385</v>
@@ -5346,128 +5333,122 @@
         <v>386</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q46" s="6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="T46" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="U46" s="6" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="V46" s="6" t="s">
-        <v>288</v>
+        <v>389</v>
       </c>
       <c r="W46" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="X46" s="6" t="s">
-        <v>360</v>
+        <v>390</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>396</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="P47" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="T47" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="V47" s="6" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="W47" s="6" t="s">
         <v>400</v>
+      </c>
+      <c r="X47" s="6" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="L48" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="K48" s="7" t="s">
+      <c r="M48" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="L48" s="13" t="s">
-        <v>406</v>
-      </c>
-      <c r="M48" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>407</v>
-      </c>
       <c r="O48" s="6" t="s">
-        <v>408</v>
+        <v>512</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>409</v>
+        <v>399</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>406</v>
       </c>
       <c r="V48" s="6" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="W48" s="6" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="X48" s="6" t="s">
         <v>205</v>
@@ -5475,55 +5456,55 @@
     </row>
     <row r="49" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="K49" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="L49" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="M49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N49" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="L49" s="8" t="s">
+      <c r="O49" s="6" t="s">
         <v>414</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="O49" s="6" t="s">
-        <v>525</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="X49" s="6" t="s">
         <v>205</v>
@@ -5531,544 +5512,538 @@
     </row>
     <row r="50" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D50" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="K50" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="L50" s="8" t="s">
         <v>418</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>422</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N50" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="P50" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S50" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="T50" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="V50" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="O50" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="P50" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="S50" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="T50" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="V50" s="6" t="s">
-        <v>399</v>
-      </c>
       <c r="W50" s="6" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>205</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D51" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>391</v>
+      <c r="G51" s="6" t="s">
+        <v>427</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="P51" s="6" t="s">
         <v>232</v>
       </c>
       <c r="S51" s="6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="V51" s="6" t="s">
-        <v>433</v>
+        <v>233</v>
       </c>
       <c r="W51" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="X51" s="6" t="s">
-        <v>399</v>
+        <v>434</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
+        <v>53</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="M52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>434</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>435</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="K52" s="7" t="s">
+      <c r="N52" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="L52" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="M52" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N52" s="6" t="s">
-        <v>440</v>
-      </c>
       <c r="O52" s="6" t="s">
-        <v>441</v>
+        <v>517</v>
       </c>
       <c r="P52" s="6" t="s">
         <v>232</v>
       </c>
+      <c r="Q52" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="S52" s="6" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="V52" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W52" s="6" t="s">
-        <v>444</v>
+        <v>434</v>
+      </c>
+      <c r="X52" s="6" t="s">
+        <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>435</v>
+        <v>248</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>437</v>
+        <v>130</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>442</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>447</v>
+        <v>520</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="P53" s="6" t="s">
         <v>232</v>
       </c>
       <c r="Q53" s="6" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="S53" s="6" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>449</v>
+        <v>444</v>
+      </c>
+      <c r="U53" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="V53" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W53" s="6" t="s">
-        <v>444</v>
+        <v>233</v>
       </c>
       <c r="X53" s="6" t="s">
-        <v>194</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="E54" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="K54" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="F54" s="6" t="s">
+      <c r="L54" s="8" t="s">
         <v>451</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="K54" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="L54" s="8" t="s">
-        <v>534</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N54" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="O54" s="6" t="s">
         <v>453</v>
-      </c>
-      <c r="O54" s="6" t="s">
-        <v>535</v>
       </c>
       <c r="P54" s="6" t="s">
         <v>232</v>
       </c>
       <c r="Q54" s="6" t="s">
-        <v>136</v>
+        <v>35</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>454</v>
       </c>
       <c r="S54" s="6" t="s">
-        <v>442</v>
+        <v>359</v>
       </c>
       <c r="T54" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="U54" s="6" t="s">
-        <v>118</v>
+        <v>455</v>
       </c>
       <c r="V54" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W54" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="X54" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="X54" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="F55" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="H55" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="K55" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="L55" s="8" t="s">
         <v>460</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>461</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N55" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="O55" s="6" t="s">
         <v>462</v>
-      </c>
-      <c r="O55" s="6" t="s">
-        <v>463</v>
       </c>
       <c r="P55" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="Q55" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R55" s="6" t="s">
+      <c r="S55" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="U55" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="T55" s="6" t="s">
-        <v>465</v>
       </c>
       <c r="V55" s="6" t="s">
         <v>233</v>
       </c>
       <c r="W55" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="X55" s="6" t="s">
-        <v>233</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>456</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>468</v>
+        <v>505</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>470</v>
+        <v>507</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>52</v>
+        <v>508</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>471</v>
+        <v>509</v>
       </c>
       <c r="O56" s="6" t="s">
-        <v>472</v>
+        <v>510</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>232</v>
       </c>
       <c r="S56" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>473</v>
+        <v>493</v>
       </c>
       <c r="U56" s="6" t="s">
-        <v>474</v>
+        <v>434</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>233</v>
+        <v>332</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>475</v>
+        <v>434</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>518</v>
+        <v>466</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>446</v>
       </c>
       <c r="K57" s="7" t="s">
-        <v>519</v>
+        <v>446</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>520</v>
+        <v>467</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>521</v>
+        <v>149</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>522</v>
+        <v>468</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>523</v>
+        <v>469</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>232</v>
+        <v>56</v>
       </c>
       <c r="S57" s="6" t="s">
-        <v>342</v>
+        <v>359</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="U57" s="6" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="V57" s="6" t="s">
-        <v>342</v>
+        <v>233</v>
       </c>
       <c r="W57" s="6" t="s">
-        <v>444</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>342</v>
+        <v>541</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>445</v>
+        <v>470</v>
       </c>
       <c r="D58" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="L58" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="M58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N58" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>456</v>
-      </c>
-      <c r="K58" s="7" t="s">
-        <v>456</v>
-      </c>
-      <c r="L58" s="8" t="s">
+      <c r="O58" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="M58" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N58" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="O58" s="6" t="s">
-        <v>479</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>56</v>
       </c>
       <c r="S58" s="6" t="s">
-        <v>369</v>
+        <v>194</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>465</v>
+        <v>478</v>
+      </c>
+      <c r="U58" s="6" t="s">
+        <v>223</v>
       </c>
       <c r="V58" s="6" t="s">
-        <v>233</v>
+        <v>423</v>
       </c>
       <c r="W58" s="6" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>342</v>
+        <v>541</v>
       </c>
       <c r="C59" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="K59" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="L59" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="F59" s="6" t="s">
+      <c r="M59" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="N59" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="K59" s="7" t="s">
+      <c r="O59" s="6" t="s">
         <v>484</v>
-      </c>
-      <c r="L59" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="M59" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="O59" s="6" t="s">
-        <v>487</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>56</v>
@@ -6077,62 +6052,12 @@
         <v>194</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="U59" s="6" t="s">
-        <v>223</v>
+        <v>485</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="W59" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>60</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>489</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>491</v>
-      </c>
-      <c r="K60" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="L60" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="M60" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="O60" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="P60" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="S60" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="T60" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="V60" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="W60" s="6" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6150,7 +6075,7 @@
     <hyperlink ref="L16" r:id="rId10" xr:uid="{273DF806-1BFB-4885-AAA0-2A07D17AEDC1}"/>
     <hyperlink ref="L17" r:id="rId11" xr:uid="{4BB0B568-E23C-4D60-BB58-2B6921573820}"/>
     <hyperlink ref="L19" r:id="rId12" xr:uid="{7977FBFE-C6C2-44B0-A7F6-04A06D6F7F49}"/>
-    <hyperlink ref="L24" r:id="rId13" display="https://faculty.dukekunshan.edu.cn/faculty_profiles/linfeng-huang" xr:uid="{69D3DB11-C5D2-4F29-B8E7-9D93439B647A}"/>
+    <hyperlink ref="L24" r:id="rId13" xr:uid="{69D3DB11-C5D2-4F29-B8E7-9D93439B647A}"/>
     <hyperlink ref="L25" r:id="rId14" xr:uid="{00A85A45-8229-4A7C-A09E-056A341C953E}"/>
     <hyperlink ref="L26" r:id="rId15" xr:uid="{F6A8F67C-D69D-407F-9920-2F13D7D2912D}"/>
     <hyperlink ref="L29" r:id="rId16" xr:uid="{523EB51B-334C-4C4D-89C5-0A1D06556799}"/>
@@ -6160,48 +6085,57 @@
     <hyperlink ref="L36" r:id="rId20" xr:uid="{289C8354-BE26-4BFC-BF0E-5D2A8D76F6AC}"/>
     <hyperlink ref="L37" r:id="rId21" xr:uid="{0DB53C1C-7BEE-4803-B673-EAF907982BA2}"/>
     <hyperlink ref="L38" r:id="rId22" xr:uid="{D969F2A3-67C8-4FC0-A967-C76E11924090}"/>
-    <hyperlink ref="L40" r:id="rId23" xr:uid="{870A9D95-1B1A-4215-B637-63206465EB5A}"/>
-    <hyperlink ref="L41" r:id="rId24" xr:uid="{77B5AA53-689F-414B-8276-18423606F312}"/>
-    <hyperlink ref="L42" r:id="rId25" xr:uid="{CB9B782F-5172-477C-A954-DD9716637CD9}"/>
-    <hyperlink ref="L43" r:id="rId26" xr:uid="{937B41B1-3682-4C5E-ADA1-D49CF763AB68}"/>
-    <hyperlink ref="L44" r:id="rId27" xr:uid="{E9DED7F2-1D8E-4D91-82EF-3D78C38F869D}"/>
-    <hyperlink ref="L47" r:id="rId28" xr:uid="{87579977-9A4C-4BE9-B612-8F7CD1AFE6CA}"/>
-    <hyperlink ref="L49" r:id="rId29" xr:uid="{2D75F78C-840B-4533-95C8-BFF7B4F68DAB}"/>
-    <hyperlink ref="L50" r:id="rId30" xr:uid="{1CB575B5-09FB-45E6-A5A4-311354A84381}"/>
-    <hyperlink ref="L52" r:id="rId31" xr:uid="{3B81BCEE-11F1-4B68-BAE0-972C7E859579}"/>
-    <hyperlink ref="L53" r:id="rId32" xr:uid="{1DCD27EC-CA22-4782-BAC7-B41C44FCFD06}"/>
-    <hyperlink ref="L55" r:id="rId33" xr:uid="{9C75757A-DE9C-4D4E-80FC-DE89C87FBD11}"/>
-    <hyperlink ref="L56" r:id="rId34" xr:uid="{0C0EC525-E23B-4660-8AAF-06AE4567BA05}"/>
-    <hyperlink ref="L58" r:id="rId35" xr:uid="{B7CDC6A2-6150-4FDA-8B01-7B1D990940B5}"/>
-    <hyperlink ref="L59" r:id="rId36" xr:uid="{D6E49538-E82F-42DC-B733-0963C1496884}"/>
-    <hyperlink ref="L45" r:id="rId37" xr:uid="{76610AF0-0460-4512-BA67-F357E14FC6E9}"/>
-    <hyperlink ref="L46" r:id="rId38" xr:uid="{81417274-1EAB-460D-9819-04C06C9D122D}"/>
-    <hyperlink ref="L54" r:id="rId39" xr:uid="{24299A3B-D828-488C-ADD2-6C63BE6E5CB8}"/>
-    <hyperlink ref="L60" r:id="rId40" xr:uid="{B0B148FB-7B5D-4FFB-BDDB-6500999AFE83}"/>
-    <hyperlink ref="L51" r:id="rId41" xr:uid="{C6C7A258-B6BD-42C1-B158-70BD7F2080AC}"/>
-    <hyperlink ref="L32" r:id="rId42" xr:uid="{C240C03B-D8F7-41E8-90EB-64AB4BEA740D}"/>
-    <hyperlink ref="L2" r:id="rId43" xr:uid="{44120993-1468-499B-998B-B5DF3DAB2FC9}"/>
-    <hyperlink ref="L4" r:id="rId44" xr:uid="{2FAFAEAA-A711-40E5-B455-A282E8D879A3}"/>
-    <hyperlink ref="L8" r:id="rId45" xr:uid="{7842F564-4B55-4539-B16B-2705C90D5A84}"/>
-    <hyperlink ref="L14" r:id="rId46" xr:uid="{96BCCCF6-F353-44FB-970E-926F50C5F7E8}"/>
-    <hyperlink ref="L18" r:id="rId47" xr:uid="{CBFC5538-0034-4703-8D79-2103DF367071}"/>
-    <hyperlink ref="L20" r:id="rId48" xr:uid="{AF24AAEC-FA13-449E-8C2F-EB83FB3D2BC2}"/>
-    <hyperlink ref="L21" r:id="rId49" xr:uid="{6DA962E4-4FED-4804-A751-2FB7466AC0B7}"/>
-    <hyperlink ref="L23" r:id="rId50" xr:uid="{987F58EB-A8CC-43FD-90AF-39AF50F1C16E}"/>
-    <hyperlink ref="L27" r:id="rId51" xr:uid="{630D6D8A-3BA0-4362-B8BF-98EA3609BF0B}"/>
-    <hyperlink ref="L30" r:id="rId52" xr:uid="{CB7B179B-C7C6-451A-AB64-76C37CBC111F}"/>
-    <hyperlink ref="L39" r:id="rId53" xr:uid="{1FCD329E-6B84-4EAA-B176-7B053A3DA255}"/>
-    <hyperlink ref="L48" r:id="rId54" xr:uid="{4C9656AE-E61B-4DFE-B3E7-7A985DB1D5D6}"/>
-    <hyperlink ref="L22" r:id="rId55" xr:uid="{5D37EC19-4EB9-4DD8-9B95-EA7F0EB869CB}"/>
-    <hyperlink ref="N28" r:id="rId56" xr:uid="{DFB81A75-9D40-4E3C-AB20-DA2B413EE03E}"/>
-    <hyperlink ref="N34" r:id="rId57" xr:uid="{C7C9B0B7-320E-4598-BE11-8BB3E848B2B7}"/>
+    <hyperlink ref="L40" r:id="rId23" xr:uid="{77B5AA53-689F-414B-8276-18423606F312}"/>
+    <hyperlink ref="L41" r:id="rId24" xr:uid="{CB9B782F-5172-477C-A954-DD9716637CD9}"/>
+    <hyperlink ref="L42" r:id="rId25" xr:uid="{937B41B1-3682-4C5E-ADA1-D49CF763AB68}"/>
+    <hyperlink ref="L43" r:id="rId26" xr:uid="{E9DED7F2-1D8E-4D91-82EF-3D78C38F869D}"/>
+    <hyperlink ref="L46" r:id="rId27" xr:uid="{87579977-9A4C-4BE9-B612-8F7CD1AFE6CA}"/>
+    <hyperlink ref="L48" r:id="rId28" xr:uid="{2D75F78C-840B-4533-95C8-BFF7B4F68DAB}"/>
+    <hyperlink ref="L49" r:id="rId29" xr:uid="{1CB575B5-09FB-45E6-A5A4-311354A84381}"/>
+    <hyperlink ref="L51" r:id="rId30" xr:uid="{3B81BCEE-11F1-4B68-BAE0-972C7E859579}"/>
+    <hyperlink ref="L52" r:id="rId31" xr:uid="{1DCD27EC-CA22-4782-BAC7-B41C44FCFD06}"/>
+    <hyperlink ref="L54" r:id="rId32" xr:uid="{9C75757A-DE9C-4D4E-80FC-DE89C87FBD11}"/>
+    <hyperlink ref="L55" r:id="rId33" xr:uid="{0C0EC525-E23B-4660-8AAF-06AE4567BA05}"/>
+    <hyperlink ref="L57" r:id="rId34" xr:uid="{B7CDC6A2-6150-4FDA-8B01-7B1D990940B5}"/>
+    <hyperlink ref="L58" r:id="rId35" xr:uid="{D6E49538-E82F-42DC-B733-0963C1496884}"/>
+    <hyperlink ref="L44" r:id="rId36" xr:uid="{76610AF0-0460-4512-BA67-F357E14FC6E9}"/>
+    <hyperlink ref="L45" r:id="rId37" xr:uid="{81417274-1EAB-460D-9819-04C06C9D122D}"/>
+    <hyperlink ref="L53" r:id="rId38" xr:uid="{24299A3B-D828-488C-ADD2-6C63BE6E5CB8}"/>
+    <hyperlink ref="L59" r:id="rId39" xr:uid="{B0B148FB-7B5D-4FFB-BDDB-6500999AFE83}"/>
+    <hyperlink ref="L50" r:id="rId40" xr:uid="{C6C7A258-B6BD-42C1-B158-70BD7F2080AC}"/>
+    <hyperlink ref="L32" r:id="rId41" xr:uid="{C240C03B-D8F7-41E8-90EB-64AB4BEA740D}"/>
+    <hyperlink ref="L2" r:id="rId42" xr:uid="{44120993-1468-499B-998B-B5DF3DAB2FC9}"/>
+    <hyperlink ref="L4" r:id="rId43" xr:uid="{2FAFAEAA-A711-40E5-B455-A282E8D879A3}"/>
+    <hyperlink ref="L8" r:id="rId44" xr:uid="{7842F564-4B55-4539-B16B-2705C90D5A84}"/>
+    <hyperlink ref="L14" r:id="rId45" xr:uid="{96BCCCF6-F353-44FB-970E-926F50C5F7E8}"/>
+    <hyperlink ref="L18" r:id="rId46" xr:uid="{CBFC5538-0034-4703-8D79-2103DF367071}"/>
+    <hyperlink ref="L20" r:id="rId47" xr:uid="{AF24AAEC-FA13-449E-8C2F-EB83FB3D2BC2}"/>
+    <hyperlink ref="L21" r:id="rId48" xr:uid="{6DA962E4-4FED-4804-A751-2FB7466AC0B7}"/>
+    <hyperlink ref="L23" r:id="rId49" xr:uid="{987F58EB-A8CC-43FD-90AF-39AF50F1C16E}"/>
+    <hyperlink ref="L27" r:id="rId50" xr:uid="{630D6D8A-3BA0-4362-B8BF-98EA3609BF0B}"/>
+    <hyperlink ref="L30" r:id="rId51" xr:uid="{CB7B179B-C7C6-451A-AB64-76C37CBC111F}"/>
+    <hyperlink ref="L39" r:id="rId52" xr:uid="{1FCD329E-6B84-4EAA-B176-7B053A3DA255}"/>
+    <hyperlink ref="L47" r:id="rId53" xr:uid="{4C9656AE-E61B-4DFE-B3E7-7A985DB1D5D6}"/>
+    <hyperlink ref="L22" r:id="rId54" xr:uid="{5D37EC19-4EB9-4DD8-9B95-EA7F0EB869CB}"/>
+    <hyperlink ref="N28" r:id="rId55" xr:uid="{DFB81A75-9D40-4E3C-AB20-DA2B413EE03E}"/>
+    <hyperlink ref="N34" r:id="rId56" xr:uid="{C7C9B0B7-320E-4598-BE11-8BB3E848B2B7}"/>
+    <hyperlink ref="L28" r:id="rId57" xr:uid="{C05D70DD-778B-40CD-A488-E1FD5DB2A553}"/>
+    <hyperlink ref="L13" r:id="rId58" xr:uid="{1EA964C8-CCEC-464F-B641-0F0EF7B76338}"/>
+    <hyperlink ref="L33" r:id="rId59" xr:uid="{7CD66981-F779-4DF4-8755-251DC16E0B34}"/>
+    <hyperlink ref="L56" r:id="rId60" xr:uid="{3651FAD9-EBC8-439D-A439-D53F93C7EECB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId61"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7A11A7DF961CC428587DE372F9C797B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4479d4a86de7b259c45e5a73c6b02c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7104dee3-b68d-4fc6-af76-78212a7605a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1efb2fb76da6e7bc543ba0de5d23ee76" ns3:_="">
     <xsd:import namespace="7104dee3-b68d-4fc6-af76-78212a7605a5"/>
@@ -6359,12 +6293,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6375,6 +6303,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B767E0B-7018-4DA6-B0B7-DFC282E8DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6392,15 +6329,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
add three new faculty info; update one faculty teaching info
</commit_message>
<xml_diff>
--- a/data_script/dku_knowledge_230504.xlsx
+++ b/data_script/dku_knowledge_230504.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sd540\Desktop\Division Portal\Interdisciplinary-Knowledge-Map-DKU\data_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://prodduke-my.sharepoint.com/personal/sd540_duke_edu/Documents/Desktop/Division Portal/Interdisciplinary-Knowledge-Map-DKU/data_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F239D-4EB9-42AB-8517-3FBF7B66E05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{6DD5927D-6119-4BBB-B892-B57BAC539348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0418E2A-05BA-413E-9801-B60E29A73838}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="559">
   <si>
     <t>id</t>
   </si>
@@ -993,9 +993,6 @@
   </si>
   <si>
     <t>domna.kotsifaki@dukekunshan.edu.cn</t>
-  </si>
-  <si>
-    <t>BIOPHYSICS</t>
   </si>
   <si>
     <t>Chemistry</t>
@@ -1679,6 +1676,57 @@
   </si>
   <si>
     <t>https://newstatic.dukekunshan.edu.cn/globalhealth/2022/05/07145949/CV-SAJID-UMAR-2022.pdf</t>
+  </si>
+  <si>
+    <t>Tongshu Zheng</t>
+  </si>
+  <si>
+    <t>tongshu.zheng@dukekunshan.edu.cn</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/tongshu-zheng</t>
+  </si>
+  <si>
+    <t>ENVIR101; ENVIR304; ENVIR402</t>
+  </si>
+  <si>
+    <t>Low-cost air quality sensors;Mobile sampling;Air pollution;Remote sensing;Machine learning</t>
+  </si>
+  <si>
+    <t>Rui Liu</t>
+  </si>
+  <si>
+    <t>rui.liu454@dukekunshan.edu.cn</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/rui-liu</t>
+  </si>
+  <si>
+    <t>Organic synthesis; Porphyrins; Photoredox catalysis; Polymer chemistry</t>
+  </si>
+  <si>
+    <t>Photophysical</t>
+  </si>
+  <si>
+    <t>Yucheng Jin</t>
+  </si>
+  <si>
+    <t>yj232@duke.edu</t>
+  </si>
+  <si>
+    <t>https://faculty.dukekunshan.edu.cn/faculty_profiles/yucheng-jin</t>
+  </si>
+  <si>
+    <t>STATS401; STATS402</t>
+  </si>
+  <si>
+    <t>Human-Computer Interaction (HCI); Human-Centered Artificial Intelligence (AI); AI for Health and Well-being; Augmented Creativity</t>
+  </si>
+  <si>
+    <t>CHEM201; CHEM150</t>
+  </si>
+  <si>
+    <t>PHYSICS</t>
   </si>
 </sst>
 </file>
@@ -2386,6 +2434,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2683,12 +2735,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2697,13 +2749,14 @@
     <col min="2" max="2" width="58.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" style="6" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
-    <col min="5" max="9" width="12.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="8" width="12.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="6" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="70.42578125" style="7" customWidth="1"/>
     <col min="12" max="12" width="84" style="6" customWidth="1"/>
     <col min="13" max="13" width="26" style="6" customWidth="1"/>
     <col min="14" max="14" width="63.85546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="81.140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="120" style="6" customWidth="1"/>
     <col min="16" max="16" width="70.42578125" style="6" customWidth="1"/>
     <col min="17" max="17" width="62.85546875" style="6" customWidth="1"/>
     <col min="18" max="18" width="43.85546875" style="6" customWidth="1"/>
@@ -2816,7 +2869,7 @@
         <v>30</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>31</v>
@@ -2878,7 +2931,7 @@
         <v>44</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>34</v>
@@ -2919,10 +2972,10 @@
         <v>49</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>50</v>
@@ -3161,7 +3214,7 @@
         <v>88</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>185</v>
@@ -3217,7 +3270,7 @@
         <v>29</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>93</v>
@@ -3229,7 +3282,7 @@
         <v>94</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>34</v>
@@ -3444,22 +3497,22 @@
         <v>25</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="K13" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="L13" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>485</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>523</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>486</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>34</v>
@@ -3474,7 +3527,7 @@
         <v>24</v>
       </c>
       <c r="X13" s="14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="12.6" customHeight="1">
@@ -3500,7 +3553,7 @@
         <v>128</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>31</v>
@@ -3509,7 +3562,7 @@
         <v>129</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>53</v>
@@ -3736,7 +3789,7 @@
         <v>162</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>31</v>
@@ -3857,7 +3910,7 @@
         <v>177</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>178</v>
@@ -3916,7 +3969,7 @@
         <v>184</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>185</v>
@@ -3925,7 +3978,7 @@
         <v>186</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>53</v>
@@ -3960,34 +4013,34 @@
         <v>124</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>108</v>
       </c>
       <c r="L22" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="M22" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="N22" s="6" t="s">
         <v>473</v>
       </c>
-      <c r="N22" s="6" t="s">
-        <v>474</v>
-      </c>
       <c r="O22" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>53</v>
       </c>
       <c r="S22" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="T22" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="T22" s="13" t="s">
+      <c r="U22" s="13" t="s">
         <v>476</v>
-      </c>
-      <c r="U22" s="13" t="s">
-        <v>477</v>
       </c>
       <c r="V22" s="6" t="s">
         <v>132</v>
@@ -4022,7 +4075,7 @@
         <v>193</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>31</v>
@@ -4078,7 +4131,7 @@
         <v>205</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>31</v>
@@ -4240,10 +4293,10 @@
         <v>230</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>31</v>
@@ -4252,7 +4305,7 @@
         <v>231</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>54</v>
@@ -4293,13 +4346,13 @@
         <v>235</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N28" s="11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>236</v>
@@ -4361,7 +4414,7 @@
         <v>243</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>50</v>
@@ -4414,10 +4467,10 @@
         <v>219</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>249</v>
@@ -4485,7 +4538,7 @@
         <v>257</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="P31" s="6" t="s">
         <v>54</v>
@@ -4567,22 +4620,22 @@
         <v>188</v>
       </c>
       <c r="D33" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="K33" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="K33" s="7" t="s">
+      <c r="L33" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="O33" s="6" t="s">
         <v>480</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>525</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>482</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>481</v>
       </c>
       <c r="P33" s="6" t="s">
         <v>54</v>
@@ -4594,7 +4647,7 @@
         <v>232</v>
       </c>
       <c r="U33" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="V33" s="6" t="s">
         <v>197</v>
@@ -4632,7 +4685,7 @@
         <v>271</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L34" s="8" t="s">
         <v>272</v>
@@ -4641,16 +4694,16 @@
         <v>273</v>
       </c>
       <c r="N34" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="O34" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="Q34" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="R34" s="6" t="s">
         <v>53</v>
@@ -4933,7 +4986,7 @@
         <v>316</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>50</v>
@@ -4942,7 +4995,7 @@
         <v>317</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>34</v>
@@ -4951,7 +5004,7 @@
         <v>54</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>318</v>
+        <v>558</v>
       </c>
       <c r="T39" s="6" t="s">
         <v>295</v>
@@ -4960,7 +5013,7 @@
         <v>197</v>
       </c>
       <c r="W39" s="6" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="X39" s="6" t="s">
         <v>277</v>
@@ -4971,37 +5024,37 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D40" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="F40" s="6" t="s">
+      <c r="G40" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="K40" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="L40" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>145</v>
       </c>
       <c r="N40" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="O40" s="6" t="s">
         <v>327</v>
-      </c>
-      <c r="O40" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>34</v>
@@ -5010,19 +5063,19 @@
         <v>54</v>
       </c>
       <c r="S40" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="T40" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="T40" s="6" t="s">
-        <v>330</v>
       </c>
       <c r="V40" s="6" t="s">
         <v>225</v>
       </c>
       <c r="W40" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X40" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="12.6" customHeight="1">
@@ -5030,37 +5083,37 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="F41" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="G41" s="6" t="s">
+      <c r="K41" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="L41" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="M41" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N41" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="O41" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="O41" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="P41" s="6" t="s">
         <v>34</v>
@@ -5069,10 +5122,10 @@
         <v>224</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="T41" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>225</v>
@@ -5089,37 +5142,37 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="G42" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="K42" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="K42" s="7" t="s">
+      <c r="L42" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>344</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N42" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="O42" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="O42" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>224</v>
@@ -5128,16 +5181,16 @@
         <v>34</v>
       </c>
       <c r="S42" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="U42" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="U42" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="V42" s="6" t="s">
         <v>276</v>
       </c>
       <c r="W42" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="12.6" customHeight="1">
@@ -5145,34 +5198,34 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>191</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M43" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N43" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="O43" s="6" t="s">
         <v>351</v>
-      </c>
-      <c r="O43" s="6" t="s">
-        <v>352</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>54</v>
@@ -5181,19 +5234,19 @@
         <v>34</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="V43" s="6" t="s">
         <v>276</v>
       </c>
       <c r="W43" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X43" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="12.6" customHeight="1">
@@ -5201,31 +5254,31 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="K44" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="L44" s="8" t="s">
         <v>356</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>357</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>145</v>
       </c>
       <c r="N44" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="O44" s="6" t="s">
         <v>358</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="P44" s="6" t="s">
         <v>224</v>
@@ -5234,22 +5287,22 @@
         <v>34</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T44" s="6" t="s">
         <v>294</v>
       </c>
       <c r="U44" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="V44" s="6" t="s">
         <v>276</v>
       </c>
       <c r="W44" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X44" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:24" ht="12.6" customHeight="1">
@@ -5257,31 +5310,31 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>266</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="K45" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="L45" s="8" t="s">
         <v>362</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>363</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N45" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="O45" s="6" t="s">
         <v>364</v>
-      </c>
-      <c r="O45" s="6" t="s">
-        <v>365</v>
       </c>
       <c r="P45" s="6" t="s">
         <v>224</v>
@@ -5290,22 +5343,22 @@
         <v>34</v>
       </c>
       <c r="S45" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="T45" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="U45" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="T45" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="U45" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="V45" s="6" t="s">
         <v>276</v>
       </c>
       <c r="W45" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X45" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="12.6" customHeight="1">
@@ -5313,52 +5366,52 @@
         <v>46</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C46" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="K46" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="K46" s="7" t="s">
+      <c r="L46" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>373</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N46" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="O46" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="O46" s="6" t="s">
-        <v>375</v>
       </c>
       <c r="P46" s="6" t="s">
         <v>54</v>
       </c>
       <c r="S46" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="T46" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="T46" s="6" t="s">
+      <c r="V46" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="V46" s="6" t="s">
+      <c r="W46" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="W46" s="6" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="12.6" customHeight="1">
@@ -5366,46 +5419,46 @@
         <v>48</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D47" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="D47" s="17" t="s">
+      <c r="E47" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="K47" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="K47" s="7" t="s">
-        <v>384</v>
-      </c>
       <c r="L47" s="16" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="M47" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N47" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="O47" s="6" t="s">
         <v>385</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>386</v>
       </c>
       <c r="P47" s="6" t="s">
         <v>54</v>
       </c>
       <c r="S47" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="V47" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="W47" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="V47" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="W47" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="X47" s="6" t="s">
         <v>197</v>
@@ -5416,52 +5469,52 @@
         <v>49</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="L48" s="8" t="s">
         <v>391</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="L48" s="8" t="s">
-        <v>392</v>
       </c>
       <c r="M48" s="6" t="s">
         <v>62</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>54</v>
       </c>
       <c r="S48" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="T48" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="V48" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="W48" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="T48" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="V48" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="W48" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="X48" s="6" t="s">
         <v>197</v>
@@ -5472,52 +5525,52 @@
         <v>50</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="K49" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="K49" s="7" t="s">
+      <c r="L49" s="8" t="s">
         <v>399</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>400</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N49" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="O49" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="O49" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>54</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="T49" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="V49" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="W49" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="X49" s="6" t="s">
         <v>197</v>
@@ -5528,52 +5581,52 @@
         <v>51</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D50" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="F50" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="K50" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>405</v>
-      </c>
       <c r="L50" s="16" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N50" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="O50" s="6" t="s">
         <v>406</v>
-      </c>
-      <c r="O50" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="P50" s="6" t="s">
         <v>224</v>
       </c>
       <c r="S50" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="T50" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="T50" s="6" t="s">
+      <c r="V50" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="V50" s="6" t="s">
-        <v>410</v>
-      </c>
       <c r="W50" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="X50" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="12.6" customHeight="1">
@@ -5581,52 +5634,52 @@
         <v>52</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="K51" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="K51" s="7" t="s">
+      <c r="L51" s="8" t="s">
         <v>415</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>416</v>
       </c>
       <c r="M51" s="6" t="s">
         <v>31</v>
       </c>
       <c r="N51" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="O51" s="6" t="s">
         <v>417</v>
-      </c>
-      <c r="O51" s="6" t="s">
-        <v>418</v>
       </c>
       <c r="P51" s="6" t="s">
         <v>224</v>
       </c>
       <c r="S51" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="T51" s="6" t="s">
         <v>419</v>
-      </c>
-      <c r="T51" s="6" t="s">
-        <v>420</v>
       </c>
       <c r="V51" s="6" t="s">
         <v>225</v>
       </c>
       <c r="W51" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="12" customHeight="1">
@@ -5634,37 +5687,37 @@
         <v>53</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C52" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="E52" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="L52" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="K52" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>424</v>
       </c>
       <c r="M52" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="P52" s="6" t="s">
         <v>224</v>
@@ -5673,16 +5726,16 @@
         <v>53</v>
       </c>
       <c r="S52" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="V52" s="6" t="s">
         <v>225</v>
       </c>
       <c r="W52" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="X52" s="6" t="s">
         <v>187</v>
@@ -5693,40 +5746,40 @@
         <v>54</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>239</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>127</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L53" s="16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P53" s="6" t="s">
         <v>224</v>
@@ -5735,10 +5788,10 @@
         <v>132</v>
       </c>
       <c r="S53" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T53" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="U53" s="6" t="s">
         <v>115</v>
@@ -5758,40 +5811,40 @@
         <v>55</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="G54" s="6" t="s">
+      <c r="H54" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="H54" s="6" t="s">
+      <c r="K54" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="L54" s="8" t="s">
         <v>437</v>
-      </c>
-      <c r="L54" s="8" t="s">
-        <v>438</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N54" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="O54" s="6" t="s">
         <v>439</v>
-      </c>
-      <c r="O54" s="6" t="s">
-        <v>440</v>
       </c>
       <c r="P54" s="6" t="s">
         <v>224</v>
@@ -5800,19 +5853,19 @@
         <v>34</v>
       </c>
       <c r="R54" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="S54" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="T54" s="6" t="s">
         <v>441</v>
-      </c>
-      <c r="S54" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="T54" s="6" t="s">
-        <v>442</v>
       </c>
       <c r="V54" s="6" t="s">
         <v>225</v>
       </c>
       <c r="W54" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="X54" s="6" t="s">
         <v>225</v>
@@ -5823,58 +5876,58 @@
         <v>56</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>443</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="G55" s="6" t="s">
+      <c r="H55" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="K55" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="L55" s="8" t="s">
         <v>446</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>447</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N55" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="O55" s="6" t="s">
         <v>448</v>
-      </c>
-      <c r="O55" s="6" t="s">
-        <v>449</v>
       </c>
       <c r="P55" s="6" t="s">
         <v>224</v>
       </c>
       <c r="S55" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T55" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="U55" s="6" t="s">
         <v>450</v>
-      </c>
-      <c r="U55" s="6" t="s">
-        <v>451</v>
       </c>
       <c r="V55" s="6" t="s">
         <v>225</v>
       </c>
       <c r="W55" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="12.6" customHeight="1">
@@ -5882,46 +5935,46 @@
         <v>57</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D56" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="K56" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="K56" s="7" t="s">
+      <c r="L56" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="M56" s="6" t="s">
         <v>491</v>
       </c>
-      <c r="L56" s="16" t="s">
-        <v>540</v>
-      </c>
-      <c r="M56" s="6" t="s">
+      <c r="N56" s="6" t="s">
         <v>492</v>
       </c>
-      <c r="N56" s="6" t="s">
+      <c r="O56" s="6" t="s">
         <v>493</v>
-      </c>
-      <c r="O56" s="6" t="s">
-        <v>494</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>224</v>
       </c>
       <c r="S56" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T56" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="U56" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="V56" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="W56" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:24" ht="12.6" customHeight="1">
@@ -5929,40 +5982,40 @@
         <v>58</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="L57" s="8" t="s">
         <v>453</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="K57" s="7" t="s">
-        <v>433</v>
-      </c>
-      <c r="L57" s="8" t="s">
-        <v>454</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>145</v>
       </c>
       <c r="N57" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="O57" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="O57" s="6" t="s">
-        <v>456</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>54</v>
       </c>
       <c r="S57" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="T57" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V57" s="6" t="s">
         <v>225</v>
@@ -5976,37 +6029,37 @@
         <v>59</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C58" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="E58" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="G58" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="K58" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="K58" s="7" t="s">
+      <c r="L58" s="8" t="s">
         <v>461</v>
-      </c>
-      <c r="L58" s="8" t="s">
-        <v>462</v>
       </c>
       <c r="M58" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N58" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="O58" s="6" t="s">
         <v>463</v>
-      </c>
-      <c r="O58" s="6" t="s">
-        <v>464</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>54</v>
@@ -6015,13 +6068,13 @@
         <v>187</v>
       </c>
       <c r="T58" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="U58" s="6" t="s">
         <v>215</v>
       </c>
       <c r="V58" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="W58" s="6" t="s">
         <v>187</v>
@@ -6032,31 +6085,31 @@
         <v>60</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D59" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>467</v>
-      </c>
       <c r="K59" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="L59" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="M59" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N59" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="O59" s="6" t="s">
         <v>468</v>
-      </c>
-      <c r="O59" s="6" t="s">
-        <v>469</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>54</v>
@@ -6065,13 +6118,154 @@
         <v>187</v>
       </c>
       <c r="T59" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="V59" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="W59" s="6" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="A60" s="5">
+        <v>61</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="L60" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N60" t="s">
+        <v>543</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="P60" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="S60" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="T60" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="U60" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="V60" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="W60" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="X60" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24">
+      <c r="A61" s="5">
+        <v>62</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="L61" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N61" t="s">
+        <v>548</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="P61" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q61" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="S61" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="U61" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="V61" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="W61" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="A62" s="5">
+        <v>63</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="K62" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="L62" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="M62" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N62" t="s">
+        <v>553</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="P62" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q62" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S62" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="T62" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="V62" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="W62" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -6137,9 +6331,12 @@
     <hyperlink ref="L33" r:id="rId58" xr:uid="{7CD66981-F779-4DF4-8755-251DC16E0B34}"/>
     <hyperlink ref="L56" r:id="rId59" display="https://cyj-environmental-microbiology-lab.webnode.page" xr:uid="{3651FAD9-EBC8-439D-A439-D53F93C7EECB}"/>
     <hyperlink ref="L59" r:id="rId60" xr:uid="{1D104106-1D35-4DDF-AF66-581DB296D3E0}"/>
+    <hyperlink ref="L60" r:id="rId61" xr:uid="{395A4FA8-B3B1-4BBD-A3CF-7BD984C03B00}"/>
+    <hyperlink ref="L61" r:id="rId62" xr:uid="{915D2671-0D47-40F2-ADE2-AADB8748EE1C}"/>
+    <hyperlink ref="L62" r:id="rId63" xr:uid="{FE570848-1515-45D4-B6EB-DB5CE5CD2364}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId61"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
 </worksheet>
 </file>
 
@@ -6153,12 +6350,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C7A11A7DF961CC428587DE372F9C797B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4479d4a86de7b259c45e5a73c6b02c5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7104dee3-b68d-4fc6-af76-78212a7605a5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1efb2fb76da6e7bc543ba0de5d23ee76" ns3:_="">
     <xsd:import namespace="7104dee3-b68d-4fc6-af76-78212a7605a5"/>
@@ -6316,6 +6507,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35BEBCFB-411F-4110-9FB1-E7A383E18372}">
   <ds:schemaRefs>
@@ -6325,15 +6522,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B767E0B-7018-4DA6-B0B7-DFC282E8DBB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6349,4 +6537,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A4A09D7-AED6-47E0-9915-07120B2255F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>